<commit_message>
oppdaterte data- og excelfiler
</commit_message>
<xml_diff>
--- a/output/Lagserien 2022 1-2. div.xlsx
+++ b/output/Lagserien 2022 1-2. div.xlsx
@@ -880,11 +880,11 @@
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>(30/13)</t>
+          <t>(30/12)</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>20198</v>
+        <v>20360</v>
       </c>
       <c r="E13" s="4" t="inlineStr">
         <is>
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>18816</v>
+        <v>18878</v>
       </c>
       <c r="E15" s="4" t="inlineStr">
         <is>
@@ -7451,11 +7451,11 @@
       </c>
       <c r="Q146" s="7" t="inlineStr">
         <is>
-          <t>Fana</t>
+          <t>Leikvang</t>
         </is>
       </c>
       <c r="R146" s="16" t="n">
-        <v>27.05</v>
+        <v>11.09</v>
       </c>
       <c r="T146" s="5" t="n"/>
     </row>
@@ -7973,11 +7973,11 @@
       </c>
       <c r="G166" s="7" t="inlineStr">
         <is>
-          <t>Oslo/Bi</t>
+          <t>Jessheim</t>
         </is>
       </c>
       <c r="H166" s="16" t="n">
-        <v>13.07</v>
+        <v>7.08</v>
       </c>
       <c r="J166" s="5" t="n"/>
       <c r="L166" s="14" t="inlineStr">
@@ -12923,25 +12923,25 @@
       </c>
       <c r="C278" s="7" t="inlineStr">
         <is>
-          <t>Jan-Olav Gullbrå Hilleren</t>
+          <t>Jesper Jensen</t>
         </is>
       </c>
       <c r="D278" s="7" t="n">
-        <v>2008</v>
+        <v>2001</v>
       </c>
       <c r="E278" s="15" t="n">
-        <v>1.41</v>
+        <v>1.55</v>
       </c>
       <c r="F278" s="7" t="n">
-        <v>246</v>
+        <v>408</v>
       </c>
       <c r="G278" s="7" t="inlineStr">
         <is>
-          <t>Byrkjelo</t>
+          <t>Ravnanger</t>
         </is>
       </c>
       <c r="H278" s="16" t="n">
-        <v>4.09</v>
+        <v>28.09</v>
       </c>
       <c r="J278" s="5" t="n"/>
       <c r="L278" s="14" t="inlineStr">
@@ -12997,11 +12997,11 @@
       </c>
       <c r="G279" s="7" t="inlineStr">
         <is>
-          <t>Askøy</t>
+          <t>Leikvang</t>
         </is>
       </c>
       <c r="H279" s="16" t="n">
-        <v>14.03</v>
+        <v>19.03</v>
       </c>
       <c r="J279" s="5" t="n"/>
       <c r="L279" s="14" t="inlineStr">
@@ -13238,7 +13238,7 @@
         </is>
       </c>
       <c r="F285" s="20" t="n">
-        <v>11255</v>
+        <v>11417</v>
       </c>
       <c r="J285" s="5" t="n"/>
       <c r="L285" s="19" t="inlineStr">
@@ -14216,7 +14216,7 @@
         </is>
       </c>
       <c r="F308" s="20" t="n">
-        <v>20198</v>
+        <v>20360</v>
       </c>
       <c r="J308" s="5" t="n"/>
       <c r="L308" s="19" t="inlineStr">
@@ -14248,7 +14248,7 @@
         </is>
       </c>
       <c r="C310" s="20" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J310" s="5" t="n"/>
       <c r="L310" s="19" t="inlineStr">
@@ -14645,25 +14645,25 @@
       </c>
       <c r="C324" s="7" t="inlineStr">
         <is>
-          <t>Oscar Sørvik Ånderå</t>
+          <t>Johannes Sandvik Bø</t>
         </is>
       </c>
       <c r="D324" s="7" t="n">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="E324" s="15" t="n">
-        <v>56.48</v>
+        <v>54.86</v>
       </c>
       <c r="F324" s="7" t="n">
-        <v>516</v>
+        <v>572</v>
       </c>
       <c r="G324" s="7" t="inlineStr">
         <is>
-          <t>Fana</t>
+          <t>Bømlo</t>
         </is>
       </c>
       <c r="H324" s="16" t="n">
-        <v>29.05</v>
+        <v>29.09</v>
       </c>
       <c r="J324" s="5" t="n"/>
       <c r="L324" s="14" t="inlineStr">
@@ -15321,7 +15321,7 @@
         </is>
       </c>
       <c r="H335" s="16" t="n">
-        <v>10.03</v>
+        <v>10.02</v>
       </c>
       <c r="J335" s="5" t="n"/>
       <c r="L335" s="14" t="inlineStr">
@@ -15386,7 +15386,7 @@
         </is>
       </c>
       <c r="F337" s="20" t="n">
-        <v>9898</v>
+        <v>9954</v>
       </c>
       <c r="J337" s="5" t="n"/>
       <c r="L337" s="19" t="inlineStr">
@@ -16290,30 +16290,30 @@
     <row r="355" ht="13" customHeight="1">
       <c r="B355" s="14" t="inlineStr">
         <is>
-          <t>60m</t>
+          <t>400m</t>
         </is>
       </c>
       <c r="C355" s="7" t="inlineStr">
         <is>
-          <t>Sander Havn Turøy</t>
+          <t>Oscar Sørvik Ånderå</t>
         </is>
       </c>
       <c r="D355" s="7" t="n">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="E355" s="15" t="n">
-        <v>7.95</v>
+        <v>56.48</v>
       </c>
       <c r="F355" s="7" t="n">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="G355" s="7" t="inlineStr">
         <is>
-          <t>Haugesund</t>
+          <t>Fana</t>
         </is>
       </c>
       <c r="H355" s="16" t="n">
-        <v>19.01</v>
+        <v>29.05</v>
       </c>
       <c r="J355" s="5" t="n"/>
       <c r="L355" s="14" t="inlineStr">
@@ -16436,7 +16436,7 @@
         </is>
       </c>
       <c r="F358" s="20" t="n">
-        <v>8918</v>
+        <v>8924</v>
       </c>
       <c r="J358" s="5" t="n"/>
       <c r="L358" s="19" t="inlineStr">
@@ -16476,7 +16476,7 @@
         </is>
       </c>
       <c r="F360" s="20" t="n">
-        <v>18816</v>
+        <v>18878</v>
       </c>
       <c r="J360" s="5" t="n"/>
       <c r="L360" s="19" t="inlineStr">
@@ -16848,7 +16848,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>IK Hind</t>
+          <t>IL Sandvin</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -16857,16 +16857,16 @@
         </is>
       </c>
       <c r="D11" s="3" t="n">
-        <v>15493</v>
+        <v>15724</v>
       </c>
       <c r="E11" s="4" t="inlineStr">
         <is>
-          <t>(2/3d)</t>
+          <t>(3/3d)</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
-          <t>Troms</t>
+          <t>Buskerud</t>
         </is>
       </c>
     </row>
@@ -16876,7 +16876,7 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>IL Sandvin</t>
+          <t>IK Hind</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -16885,16 +16885,16 @@
         </is>
       </c>
       <c r="D12" s="3" t="n">
-        <v>15250</v>
+        <v>15493</v>
       </c>
       <c r="E12" s="4" t="inlineStr">
         <is>
-          <t>(3/3d)</t>
+          <t>(2/3d)</t>
         </is>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
-          <t>Buskerud</t>
+          <t>Troms</t>
         </is>
       </c>
     </row>
@@ -16937,11 +16937,11 @@
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>(25/11)</t>
+          <t>(25/10)</t>
         </is>
       </c>
       <c r="D14" s="3" t="n">
-        <v>13541</v>
+        <v>13711</v>
       </c>
       <c r="E14" s="4" t="inlineStr">
         <is>
@@ -24774,7 +24774,7 @@
       </c>
       <c r="C190" s="7" t="inlineStr">
         <is>
-          <t>Troms</t>
+          <t>Buskerud</t>
         </is>
       </c>
       <c r="F190" s="8" t="n">
@@ -24788,7 +24788,7 @@
       </c>
       <c r="M190" s="7" t="inlineStr">
         <is>
-          <t>Buskerud</t>
+          <t>Troms</t>
         </is>
       </c>
       <c r="P190" s="8" t="n">
@@ -24804,7 +24804,7 @@
       </c>
       <c r="C191" s="7" t="inlineStr">
         <is>
-          <t>IK Hind</t>
+          <t>IL Sandvin</t>
         </is>
       </c>
       <c r="J191" s="5" t="n"/>
@@ -24815,7 +24815,7 @@
       </c>
       <c r="M191" s="7" t="inlineStr">
         <is>
-          <t>IL Sandvin</t>
+          <t>IK Hind</t>
         </is>
       </c>
       <c r="T191" s="5" t="n"/>
@@ -24939,138 +24939,138 @@
     <row r="197" ht="13" customHeight="1">
       <c r="B197" s="14" t="inlineStr">
         <is>
-          <t>100m</t>
+          <t>60m</t>
         </is>
       </c>
       <c r="C197" s="7" t="inlineStr">
         <is>
-          <t>Birk Arvola</t>
+          <t>Sondre Witzøe</t>
         </is>
       </c>
       <c r="D197" s="7" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="E197" s="15" t="n">
-        <v>11.87</v>
+        <v>7.14</v>
       </c>
       <c r="F197" s="7" t="n">
-        <v>638</v>
+        <v>802</v>
       </c>
       <c r="G197" s="7" t="inlineStr">
         <is>
-          <t>Sortland</t>
+          <t>Steinkjer</t>
         </is>
       </c>
       <c r="H197" s="16" t="n">
-        <v>20.08</v>
+        <v>5.03</v>
       </c>
       <c r="J197" s="5" t="n"/>
       <c r="L197" s="14" t="inlineStr">
         <is>
-          <t>60m</t>
+          <t>100m</t>
         </is>
       </c>
       <c r="M197" s="7" t="inlineStr">
         <is>
-          <t>Alexander Tomala</t>
+          <t>Birk Arvola</t>
         </is>
       </c>
       <c r="N197" s="7" t="n">
         <v>2005</v>
       </c>
       <c r="O197" s="15" t="n">
-        <v>7.33</v>
+        <v>11.87</v>
       </c>
       <c r="P197" s="7" t="n">
-        <v>725</v>
+        <v>638</v>
       </c>
       <c r="Q197" s="7" t="inlineStr">
         <is>
-          <t>Bærum</t>
+          <t>Sortland</t>
         </is>
       </c>
       <c r="R197" s="16" t="n">
-        <v>12.02</v>
+        <v>20.08</v>
       </c>
       <c r="T197" s="5" t="n"/>
     </row>
     <row r="198" ht="13" customHeight="1">
       <c r="B198" s="14" t="inlineStr">
         <is>
-          <t>200m</t>
+          <t>100m</t>
         </is>
       </c>
       <c r="C198" s="7" t="inlineStr">
         <is>
-          <t>Tobias Johansen</t>
+          <t>Sondre Witzøe</t>
         </is>
       </c>
       <c r="D198" s="7" t="n">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="E198" s="15" t="n">
-        <v>22.64</v>
+        <v>10.94</v>
       </c>
       <c r="F198" s="7" t="n">
-        <v>788</v>
+        <v>857</v>
       </c>
       <c r="G198" s="7" t="inlineStr">
         <is>
-          <t>Sortland</t>
+          <t>Trondheim</t>
         </is>
       </c>
       <c r="H198" s="16" t="n">
-        <v>21.08</v>
+        <v>12.08</v>
       </c>
       <c r="J198" s="5" t="n"/>
       <c r="L198" s="14" t="inlineStr">
         <is>
-          <t>100m</t>
+          <t>200m</t>
         </is>
       </c>
       <c r="M198" s="7" t="inlineStr">
         <is>
-          <t>Sondre Witzøe</t>
+          <t>Tobias Johansen</t>
         </is>
       </c>
       <c r="N198" s="7" t="n">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="O198" s="15" t="n">
-        <v>10.94</v>
+        <v>22.64</v>
       </c>
       <c r="P198" s="7" t="n">
-        <v>857</v>
+        <v>788</v>
       </c>
       <c r="Q198" s="7" t="inlineStr">
         <is>
-          <t>Trondheim</t>
+          <t>Sortland</t>
         </is>
       </c>
       <c r="R198" s="16" t="n">
-        <v>12.08</v>
+        <v>21.08</v>
       </c>
       <c r="T198" s="5" t="n"/>
     </row>
     <row r="199" ht="13" customHeight="1">
       <c r="B199" s="14" t="inlineStr">
         <is>
-          <t>400m</t>
+          <t>200m</t>
         </is>
       </c>
       <c r="C199" s="7" t="inlineStr">
         <is>
-          <t>Tobias Johansen</t>
+          <t>Sondre Witzøe</t>
         </is>
       </c>
       <c r="D199" s="7" t="n">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="E199" s="15" t="n">
-        <v>48.92</v>
+        <v>22.45</v>
       </c>
       <c r="F199" s="7" t="n">
-        <v>841</v>
+        <v>809</v>
       </c>
       <c r="G199" s="7" t="inlineStr">
         <is>
@@ -25078,27 +25078,27 @@
         </is>
       </c>
       <c r="H199" s="16" t="n">
-        <v>27.08</v>
+        <v>28.08</v>
       </c>
       <c r="J199" s="5" t="n"/>
       <c r="L199" s="14" t="inlineStr">
         <is>
-          <t>200m</t>
+          <t>400m</t>
         </is>
       </c>
       <c r="M199" s="7" t="inlineStr">
         <is>
-          <t>Sondre Witzøe</t>
+          <t>Tobias Johansen</t>
         </is>
       </c>
       <c r="N199" s="7" t="n">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="O199" s="15" t="n">
-        <v>22.45</v>
+        <v>48.92</v>
       </c>
       <c r="P199" s="7" t="n">
-        <v>809</v>
+        <v>841</v>
       </c>
       <c r="Q199" s="7" t="inlineStr">
         <is>
@@ -25106,603 +25106,605 @@
         </is>
       </c>
       <c r="R199" s="16" t="n">
-        <v>28.08</v>
+        <v>27.08</v>
       </c>
       <c r="T199" s="5" t="n"/>
     </row>
     <row r="200" ht="13" customHeight="1">
       <c r="B200" s="14" t="inlineStr">
         <is>
-          <t>800m</t>
+          <t>400m</t>
         </is>
       </c>
       <c r="C200" s="7" t="inlineStr">
         <is>
-          <t>Tobias Johansen</t>
+          <t>Simen Johan Teigstad</t>
         </is>
       </c>
       <c r="D200" s="7" t="n">
-        <v>2003</v>
-      </c>
-      <c r="E200" s="17" t="inlineStr">
-        <is>
-          <t>1,55,51</t>
-        </is>
+        <v>2005</v>
+      </c>
+      <c r="E200" s="15" t="n">
+        <v>52.91</v>
       </c>
       <c r="F200" s="7" t="n">
-        <v>782</v>
+        <v>648</v>
       </c>
       <c r="G200" s="7" t="inlineStr">
         <is>
-          <t>Trondheim</t>
+          <t>Hamar</t>
         </is>
       </c>
       <c r="H200" s="16" t="n">
-        <v>14.08</v>
+        <v>21.05</v>
       </c>
       <c r="J200" s="5" t="n"/>
       <c r="L200" s="14" t="inlineStr">
         <is>
-          <t>400m</t>
+          <t>800m</t>
         </is>
       </c>
       <c r="M200" s="7" t="inlineStr">
         <is>
-          <t>Simen Johan Teigstad</t>
+          <t>Tobias Johansen</t>
         </is>
       </c>
       <c r="N200" s="7" t="n">
-        <v>2005</v>
-      </c>
-      <c r="O200" s="15" t="n">
-        <v>52.91</v>
+        <v>2003</v>
+      </c>
+      <c r="O200" s="17" t="inlineStr">
+        <is>
+          <t>1,55,51</t>
+        </is>
       </c>
       <c r="P200" s="7" t="n">
-        <v>648</v>
+        <v>782</v>
       </c>
       <c r="Q200" s="7" t="inlineStr">
         <is>
-          <t>Hamar</t>
+          <t>Trondheim</t>
         </is>
       </c>
       <c r="R200" s="16" t="n">
-        <v>21.05</v>
+        <v>14.08</v>
       </c>
       <c r="T200" s="5" t="n"/>
     </row>
     <row r="201" ht="13" customHeight="1">
       <c r="B201" s="14" t="inlineStr">
         <is>
-          <t>1500m</t>
+          <t>800m</t>
         </is>
       </c>
       <c r="C201" s="7" t="inlineStr">
         <is>
-          <t>Per-Christian Myrnes Pedersen</t>
+          <t>Tobias Kalmo Thorbjørnsen</t>
         </is>
       </c>
       <c r="D201" s="7" t="n">
-        <v>1986</v>
+        <v>2006</v>
       </c>
       <c r="E201" s="17" t="inlineStr">
         <is>
-          <t>4,25,41</t>
+          <t>2,26,47</t>
         </is>
       </c>
       <c r="F201" s="7" t="n">
-        <v>556</v>
+        <v>331</v>
       </c>
       <c r="G201" s="7" t="inlineStr">
         <is>
-          <t>Harstad</t>
+          <t>Sande</t>
         </is>
       </c>
       <c r="H201" s="16" t="n">
-        <v>20.09</v>
+        <v>24.09</v>
       </c>
       <c r="J201" s="5" t="n"/>
       <c r="L201" s="14" t="inlineStr">
         <is>
-          <t>800m</t>
+          <t>1500m</t>
         </is>
       </c>
       <c r="M201" s="7" t="inlineStr">
         <is>
-          <t>Tobias Kalmo Thorbjørnsen</t>
+          <t>Per-Christian Myrnes Pedersen</t>
         </is>
       </c>
       <c r="N201" s="7" t="n">
-        <v>2006</v>
+        <v>1986</v>
       </c>
       <c r="O201" s="17" t="inlineStr">
         <is>
-          <t>2,26,47</t>
+          <t>4,25,41</t>
         </is>
       </c>
       <c r="P201" s="7" t="n">
-        <v>331</v>
+        <v>556</v>
       </c>
       <c r="Q201" s="7" t="inlineStr">
         <is>
-          <t>Sande</t>
+          <t>Harstad</t>
         </is>
       </c>
       <c r="R201" s="16" t="n">
-        <v>24.09</v>
+        <v>20.09</v>
       </c>
       <c r="T201" s="5" t="n"/>
     </row>
     <row r="202" ht="13" customHeight="1">
       <c r="B202" s="14" t="inlineStr">
         <is>
-          <t>3000m</t>
+          <t>1500m</t>
         </is>
       </c>
       <c r="C202" s="7" t="inlineStr">
         <is>
-          <t>Stian Markussen Eilertsen</t>
+          <t>Simen Johan Teigstad</t>
         </is>
       </c>
       <c r="D202" s="7" t="n">
-        <v>1986</v>
+        <v>2005</v>
       </c>
       <c r="E202" s="17" t="inlineStr">
         <is>
-          <t>9,00,52</t>
+          <t>4,42,31</t>
         </is>
       </c>
       <c r="F202" s="7" t="n">
-        <v>686</v>
+        <v>449</v>
       </c>
       <c r="G202" s="7" t="inlineStr">
         <is>
-          <t>Tromsø</t>
+          <t>Hamar</t>
         </is>
       </c>
       <c r="H202" s="16" t="n">
-        <v>18.05</v>
+        <v>22.05</v>
       </c>
       <c r="J202" s="5" t="n"/>
       <c r="L202" s="14" t="inlineStr">
         <is>
-          <t>1500m</t>
+          <t>3000m</t>
         </is>
       </c>
       <c r="M202" s="7" t="inlineStr">
         <is>
-          <t>Haakon Alexander Kollerud Johansen</t>
+          <t>Stian Markussen Eilertsen</t>
         </is>
       </c>
       <c r="N202" s="7" t="n">
-        <v>2008</v>
+        <v>1986</v>
       </c>
       <c r="O202" s="17" t="inlineStr">
         <is>
-          <t>4,50,7</t>
+          <t>9,00,52</t>
         </is>
       </c>
       <c r="P202" s="7" t="n">
-        <v>401</v>
+        <v>686</v>
       </c>
       <c r="Q202" s="7" t="inlineStr">
         <is>
-          <t>Drammen</t>
+          <t>Tromsø</t>
         </is>
       </c>
       <c r="R202" s="16" t="n">
-        <v>21.08</v>
+        <v>18.05</v>
       </c>
       <c r="T202" s="5" t="n"/>
     </row>
     <row r="203" ht="13" customHeight="1">
       <c r="B203" s="14" t="inlineStr">
         <is>
-          <t>5000m</t>
+          <t>3000m</t>
         </is>
       </c>
       <c r="C203" s="7" t="inlineStr">
         <is>
-          <t>Stian Markussen Eilertsen</t>
+          <t>Tobias Kalmo Thorbjørnsen</t>
         </is>
       </c>
       <c r="D203" s="7" t="n">
-        <v>1986</v>
+        <v>2006</v>
       </c>
       <c r="E203" s="17" t="inlineStr">
         <is>
-          <t>15,44,16</t>
+          <t>11,21,07</t>
         </is>
       </c>
       <c r="F203" s="7" t="n">
-        <v>677</v>
+        <v>287</v>
       </c>
       <c r="G203" s="7" t="inlineStr">
         <is>
-          <t>Harstad</t>
+          <t>Sande</t>
         </is>
       </c>
       <c r="H203" s="16" t="n">
-        <v>24.05</v>
+        <v>1.1</v>
       </c>
       <c r="J203" s="5" t="n"/>
       <c r="L203" s="14" t="inlineStr">
         <is>
-          <t>Høyde</t>
+          <t>5000m</t>
         </is>
       </c>
       <c r="M203" s="7" t="inlineStr">
         <is>
-          <t>Simen Johan Teigstad</t>
+          <t>Stian Markussen Eilertsen</t>
         </is>
       </c>
       <c r="N203" s="7" t="n">
-        <v>2005</v>
-      </c>
-      <c r="O203" s="15" t="n">
-        <v>1.83</v>
+        <v>1986</v>
+      </c>
+      <c r="O203" s="17" t="inlineStr">
+        <is>
+          <t>15,44,16</t>
+        </is>
       </c>
       <c r="P203" s="7" t="n">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="Q203" s="7" t="inlineStr">
         <is>
-          <t>Trondheim</t>
+          <t>Harstad</t>
         </is>
       </c>
       <c r="R203" s="16" t="n">
-        <v>13.08</v>
+        <v>24.05</v>
       </c>
       <c r="T203" s="5" t="n"/>
     </row>
     <row r="204" ht="13" customHeight="1">
       <c r="B204" s="14" t="inlineStr">
         <is>
-          <t>10000m</t>
+          <t>Høyde</t>
         </is>
       </c>
       <c r="C204" s="7" t="inlineStr">
         <is>
-          <t>Erik Fossen Nilsen</t>
+          <t>Simen Johan Teigstad</t>
         </is>
       </c>
       <c r="D204" s="7" t="n">
-        <v>1987</v>
-      </c>
-      <c r="E204" s="17" t="inlineStr">
-        <is>
-          <t>33,36,42</t>
-        </is>
+        <v>2005</v>
+      </c>
+      <c r="E204" s="15" t="n">
+        <v>1.83</v>
       </c>
       <c r="F204" s="7" t="n">
-        <v>648</v>
+        <v>678</v>
       </c>
       <c r="G204" s="7" t="inlineStr">
         <is>
-          <t>Stjørdal</t>
+          <t>Trondheim</t>
         </is>
       </c>
       <c r="H204" s="16" t="n">
-        <v>26.06</v>
+        <v>13.08</v>
       </c>
       <c r="J204" s="5" t="n"/>
       <c r="L204" s="14" t="inlineStr">
         <is>
-          <t>Stav</t>
+          <t>10000m</t>
         </is>
       </c>
       <c r="M204" s="7" t="inlineStr">
         <is>
-          <t>Simen Johan Teigstad</t>
+          <t>Erik Fossen Nilsen</t>
         </is>
       </c>
       <c r="N204" s="7" t="n">
-        <v>2005</v>
-      </c>
-      <c r="O204" s="15" t="n">
-        <v>4.3</v>
+        <v>1987</v>
+      </c>
+      <c r="O204" s="17" t="inlineStr">
+        <is>
+          <t>33,36,42</t>
+        </is>
       </c>
       <c r="P204" s="7" t="n">
-        <v>777</v>
+        <v>648</v>
       </c>
       <c r="Q204" s="7" t="inlineStr">
         <is>
-          <t>Bærum</t>
+          <t>Stjørdal</t>
         </is>
       </c>
       <c r="R204" s="16" t="n">
-        <v>23.01</v>
+        <v>26.06</v>
       </c>
       <c r="T204" s="5" t="n"/>
     </row>
     <row r="205" ht="13" customHeight="1">
       <c r="B205" s="14" t="inlineStr">
         <is>
-          <t>400m hekk</t>
+          <t>Stav</t>
         </is>
       </c>
       <c r="C205" s="7" t="inlineStr">
         <is>
-          <t>Kristian Sheath</t>
+          <t>Simen Johan Teigstad</t>
         </is>
       </c>
       <c r="D205" s="7" t="n">
         <v>2005</v>
       </c>
-      <c r="E205" s="17" t="inlineStr">
-        <is>
-          <t>1,02,75</t>
-        </is>
+      <c r="E205" s="15" t="n">
+        <v>4.3</v>
       </c>
       <c r="F205" s="7" t="n">
-        <v>557</v>
+        <v>777</v>
       </c>
       <c r="G205" s="7" t="inlineStr">
         <is>
-          <t>Tromsø</t>
+          <t>Bærum</t>
         </is>
       </c>
       <c r="H205" s="16" t="n">
-        <v>3.09</v>
+        <v>23.01</v>
       </c>
       <c r="J205" s="5" t="n"/>
       <c r="L205" s="14" t="inlineStr">
         <is>
-          <t>Lengde</t>
+          <t>400m hekk</t>
         </is>
       </c>
       <c r="M205" s="7" t="inlineStr">
         <is>
-          <t>Simen Johan Teigstad</t>
+          <t>Kristian Sheath</t>
         </is>
       </c>
       <c r="N205" s="7" t="n">
         <v>2005</v>
       </c>
-      <c r="O205" s="15" t="n">
-        <v>6.47</v>
+      <c r="O205" s="17" t="inlineStr">
+        <is>
+          <t>1,02,75</t>
+        </is>
       </c>
       <c r="P205" s="7" t="n">
-        <v>712</v>
+        <v>557</v>
       </c>
       <c r="Q205" s="7" t="inlineStr">
         <is>
-          <t>Hamar</t>
+          <t>Tromsø</t>
         </is>
       </c>
       <c r="R205" s="16" t="n">
-        <v>21.05</v>
+        <v>3.09</v>
       </c>
       <c r="T205" s="5" t="n"/>
     </row>
     <row r="206" ht="13" customHeight="1">
       <c r="B206" s="14" t="inlineStr">
         <is>
-          <t>Høyde</t>
+          <t>Lengde</t>
         </is>
       </c>
       <c r="C206" s="7" t="inlineStr">
         <is>
-          <t>Mathias Johansen</t>
+          <t>Simen Johan Teigstad</t>
         </is>
       </c>
       <c r="D206" s="7" t="n">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="E206" s="15" t="n">
-        <v>1.57</v>
+        <v>6.47</v>
       </c>
       <c r="F206" s="7" t="n">
-        <v>429</v>
+        <v>712</v>
       </c>
       <c r="G206" s="7" t="inlineStr">
         <is>
-          <t>Harstad</t>
+          <t>Hamar</t>
         </is>
       </c>
       <c r="H206" s="16" t="n">
-        <v>10.09</v>
+        <v>21.05</v>
       </c>
       <c r="J206" s="5" t="n"/>
       <c r="L206" s="14" t="inlineStr">
         <is>
-          <t>Tresteg</t>
+          <t>Høyde</t>
         </is>
       </c>
       <c r="M206" s="7" t="inlineStr">
         <is>
-          <t>Tobias Kalmo Thorbjørnsen</t>
+          <t>Mathias Johansen</t>
         </is>
       </c>
       <c r="N206" s="7" t="n">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="O206" s="15" t="n">
-        <v>10.65</v>
+        <v>1.57</v>
       </c>
       <c r="P206" s="7" t="n">
-        <v>407</v>
+        <v>429</v>
       </c>
       <c r="Q206" s="7" t="inlineStr">
         <is>
-          <t>Steinkjer</t>
+          <t>Harstad</t>
         </is>
       </c>
       <c r="R206" s="16" t="n">
-        <v>4.03</v>
+        <v>10.09</v>
       </c>
       <c r="T206" s="5" t="n"/>
     </row>
     <row r="207" ht="13" customHeight="1">
       <c r="B207" s="14" t="inlineStr">
         <is>
-          <t>Lengde</t>
+          <t>Tresteg</t>
         </is>
       </c>
       <c r="C207" s="7" t="inlineStr">
         <is>
-          <t>Tobias Johansen</t>
+          <t>Tobias Kalmo Thorbjørnsen</t>
         </is>
       </c>
       <c r="D207" s="7" t="n">
-        <v>2003</v>
+        <v>2006</v>
       </c>
       <c r="E207" s="15" t="n">
-        <v>5.93</v>
+        <v>10.65</v>
       </c>
       <c r="F207" s="7" t="n">
-        <v>590</v>
+        <v>407</v>
       </c>
       <c r="G207" s="7" t="inlineStr">
         <is>
-          <t>Harstad</t>
+          <t>Steinkjer</t>
         </is>
       </c>
       <c r="H207" s="16" t="n">
-        <v>11.09</v>
+        <v>4.03</v>
       </c>
       <c r="J207" s="5" t="n"/>
       <c r="L207" s="14" t="inlineStr">
         <is>
-          <t>Høyde u.t</t>
+          <t>Lengde</t>
         </is>
       </c>
       <c r="M207" s="7" t="inlineStr">
         <is>
-          <t>Sondre Witzøe</t>
+          <t>Tobias Johansen</t>
         </is>
       </c>
       <c r="N207" s="7" t="n">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="O207" s="15" t="n">
-        <v>1.3</v>
+        <v>5.93</v>
       </c>
       <c r="P207" s="7" t="n">
-        <v>440</v>
+        <v>590</v>
       </c>
       <c r="Q207" s="7" t="inlineStr">
         <is>
-          <t>Drammen</t>
+          <t>Harstad</t>
         </is>
       </c>
       <c r="R207" s="16" t="n">
-        <v>22.03</v>
+        <v>11.09</v>
       </c>
       <c r="T207" s="5" t="n"/>
     </row>
     <row r="208" ht="13" customHeight="1">
       <c r="B208" s="14" t="inlineStr">
         <is>
-          <t>Tresteg</t>
+          <t>Lengde u.t</t>
         </is>
       </c>
       <c r="C208" s="7" t="inlineStr">
         <is>
-          <t>Tobias Johansen</t>
+          <t>Sondre Witzøe</t>
         </is>
       </c>
       <c r="D208" s="7" t="n">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="E208" s="15" t="n">
-        <v>12.48</v>
+        <v>3.03</v>
       </c>
       <c r="F208" s="7" t="n">
-        <v>613</v>
+        <v>688</v>
       </c>
       <c r="G208" s="7" t="inlineStr">
         <is>
-          <t>Harstad</t>
+          <t>Drammen</t>
         </is>
       </c>
       <c r="H208" s="16" t="n">
-        <v>10.09</v>
+        <v>22.03</v>
       </c>
       <c r="J208" s="5" t="n"/>
       <c r="L208" s="14" t="inlineStr">
         <is>
-          <t>Lengde u.t</t>
+          <t>Tresteg</t>
         </is>
       </c>
       <c r="M208" s="7" t="inlineStr">
         <is>
-          <t>Sondre Witzøe</t>
+          <t>Tobias Johansen</t>
         </is>
       </c>
       <c r="N208" s="7" t="n">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="O208" s="15" t="n">
-        <v>3.03</v>
+        <v>12.48</v>
       </c>
       <c r="P208" s="7" t="n">
-        <v>688</v>
+        <v>613</v>
       </c>
       <c r="Q208" s="7" t="inlineStr">
         <is>
-          <t>Drammen</t>
+          <t>Harstad</t>
         </is>
       </c>
       <c r="R208" s="16" t="n">
-        <v>22.03</v>
+        <v>10.09</v>
       </c>
       <c r="T208" s="5" t="n"/>
     </row>
     <row r="209" ht="13" customHeight="1">
       <c r="B209" s="14" t="inlineStr">
         <is>
-          <t>Lengde u.t</t>
+          <t>Diskos</t>
         </is>
       </c>
       <c r="C209" s="7" t="inlineStr">
         <is>
-          <t>Oskar Stattin</t>
+          <t>Fredrik Simensen</t>
         </is>
       </c>
       <c r="D209" s="7" t="n">
-        <v>2006</v>
+        <v>1992</v>
       </c>
       <c r="E209" s="15" t="n">
-        <v>2.72</v>
+        <v>37.71</v>
       </c>
       <c r="F209" s="7" t="n">
-        <v>515</v>
+        <v>642</v>
       </c>
       <c r="G209" s="7" t="inlineStr">
         <is>
-          <t>Bærum</t>
+          <t>Sande</t>
         </is>
       </c>
       <c r="H209" s="16" t="n">
-        <v>12.02</v>
+        <v>30.09</v>
       </c>
       <c r="J209" s="5" t="n"/>
       <c r="L209" s="14" t="inlineStr">
         <is>
-          <t>Spyd</t>
+          <t>Lengde u.t</t>
         </is>
       </c>
       <c r="M209" s="7" t="inlineStr">
         <is>
-          <t>Sondre Witzøe</t>
+          <t>Oskar Stattin</t>
         </is>
       </c>
       <c r="N209" s="7" t="n">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="O209" s="15" t="n">
-        <v>33.66</v>
+        <v>2.72</v>
       </c>
       <c r="P209" s="7" t="n">
-        <v>390</v>
+        <v>515</v>
       </c>
       <c r="Q209" s="7" t="inlineStr">
         <is>
-          <t>Sande</t>
+          <t>Bærum</t>
         </is>
       </c>
       <c r="R209" s="16" t="n">
-        <v>24.09</v>
+        <v>12.02</v>
       </c>
       <c r="T209" s="5" t="n"/>
     </row>
@@ -25739,7 +25741,7 @@
         </is>
       </c>
       <c r="F211" s="20" t="n">
-        <v>8320</v>
+        <v>8087</v>
       </c>
       <c r="J211" s="5" t="n"/>
       <c r="L211" s="19" t="inlineStr">
@@ -25756,7 +25758,7 @@
         </is>
       </c>
       <c r="P211" s="20" t="n">
-        <v>7863</v>
+        <v>8320</v>
       </c>
       <c r="T211" s="5" t="n"/>
     </row>
@@ -25864,25 +25866,25 @@
       </c>
       <c r="C216" s="7" t="inlineStr">
         <is>
-          <t>Birk Arvola</t>
+          <t>Alexander Tomala</t>
         </is>
       </c>
       <c r="D216" s="7" t="n">
         <v>2005</v>
       </c>
       <c r="E216" s="15" t="n">
-        <v>23.6</v>
+        <v>23.01</v>
       </c>
       <c r="F216" s="7" t="n">
-        <v>687</v>
+        <v>747</v>
       </c>
       <c r="G216" s="7" t="inlineStr">
         <is>
-          <t>Steinkjer</t>
+          <t>Bærum</t>
         </is>
       </c>
       <c r="H216" s="16" t="n">
-        <v>6.03</v>
+        <v>13.02</v>
       </c>
       <c r="J216" s="5" t="n"/>
       <c r="L216" s="14" t="inlineStr">
@@ -25892,525 +25894,525 @@
       </c>
       <c r="M216" s="7" t="inlineStr">
         <is>
-          <t>Alexander Tomala</t>
+          <t>Birk Arvola</t>
         </is>
       </c>
       <c r="N216" s="7" t="n">
         <v>2005</v>
       </c>
       <c r="O216" s="15" t="n">
-        <v>23.01</v>
+        <v>23.6</v>
       </c>
       <c r="P216" s="7" t="n">
-        <v>747</v>
+        <v>687</v>
       </c>
       <c r="Q216" s="7" t="inlineStr">
         <is>
-          <t>Bærum</t>
+          <t>Steinkjer</t>
         </is>
       </c>
       <c r="R216" s="16" t="n">
-        <v>13.02</v>
+        <v>6.03</v>
       </c>
       <c r="T216" s="5" t="n"/>
     </row>
     <row r="217" ht="13" customHeight="1">
       <c r="B217" s="14" t="inlineStr">
         <is>
-          <t>5000m</t>
+          <t>60m</t>
         </is>
       </c>
       <c r="C217" s="7" t="inlineStr">
         <is>
-          <t>Erik Fossen Nilsen</t>
+          <t>Alexander Tomala</t>
         </is>
       </c>
       <c r="D217" s="7" t="n">
-        <v>1987</v>
-      </c>
-      <c r="E217" s="17" t="inlineStr">
-        <is>
-          <t>15,48,92</t>
-        </is>
+        <v>2005</v>
+      </c>
+      <c r="E217" s="15" t="n">
+        <v>7.33</v>
       </c>
       <c r="F217" s="7" t="n">
-        <v>668</v>
+        <v>725</v>
       </c>
       <c r="G217" s="7" t="inlineStr">
         <is>
-          <t>Oslo/Bi</t>
+          <t>Bærum</t>
         </is>
       </c>
       <c r="H217" s="16" t="n">
-        <v>30.06</v>
+        <v>12.02</v>
       </c>
       <c r="J217" s="5" t="n"/>
       <c r="L217" s="14" t="inlineStr">
         <is>
-          <t>200m</t>
+          <t>5000m</t>
         </is>
       </c>
       <c r="M217" s="7" t="inlineStr">
         <is>
-          <t>Oliver Tomala</t>
+          <t>Erik Fossen Nilsen</t>
         </is>
       </c>
       <c r="N217" s="7" t="n">
-        <v>2007</v>
-      </c>
-      <c r="O217" s="15" t="n">
-        <v>23.37</v>
+        <v>1987</v>
+      </c>
+      <c r="O217" s="17" t="inlineStr">
+        <is>
+          <t>15,48,92</t>
+        </is>
       </c>
       <c r="P217" s="7" t="n">
-        <v>710</v>
+        <v>668</v>
       </c>
       <c r="Q217" s="7" t="inlineStr">
         <is>
-          <t>Trondheim</t>
+          <t>Oslo/Bi</t>
         </is>
       </c>
       <c r="R217" s="16" t="n">
-        <v>14.08</v>
+        <v>30.06</v>
       </c>
       <c r="T217" s="5" t="n"/>
     </row>
     <row r="218" ht="13" customHeight="1">
       <c r="B218" s="14" t="inlineStr">
         <is>
-          <t>5000m</t>
+          <t>200m</t>
         </is>
       </c>
       <c r="C218" s="7" t="inlineStr">
         <is>
-          <t>Per-Christian Myrnes Pedersen</t>
+          <t>Oliver Tomala</t>
         </is>
       </c>
       <c r="D218" s="7" t="n">
-        <v>1986</v>
-      </c>
-      <c r="E218" s="17" t="inlineStr">
-        <is>
-          <t>15,52,67</t>
-        </is>
+        <v>2007</v>
+      </c>
+      <c r="E218" s="15" t="n">
+        <v>23.37</v>
       </c>
       <c r="F218" s="7" t="n">
-        <v>660</v>
+        <v>710</v>
       </c>
       <c r="G218" s="7" t="inlineStr">
         <is>
-          <t>Oslo/Bi</t>
+          <t>Trondheim</t>
         </is>
       </c>
       <c r="H218" s="16" t="n">
-        <v>13.07</v>
+        <v>14.08</v>
       </c>
       <c r="J218" s="5" t="n"/>
       <c r="L218" s="14" t="inlineStr">
         <is>
-          <t>100m</t>
+          <t>5000m</t>
         </is>
       </c>
       <c r="M218" s="7" t="inlineStr">
         <is>
-          <t>Oliver Tomala</t>
+          <t>Per-Christian Myrnes Pedersen</t>
         </is>
       </c>
       <c r="N218" s="7" t="n">
-        <v>2007</v>
-      </c>
-      <c r="O218" s="15" t="n">
-        <v>11.64</v>
+        <v>1986</v>
+      </c>
+      <c r="O218" s="17" t="inlineStr">
+        <is>
+          <t>15,52,67</t>
+        </is>
       </c>
       <c r="P218" s="7" t="n">
-        <v>688</v>
+        <v>660</v>
       </c>
       <c r="Q218" s="7" t="inlineStr">
         <is>
-          <t>Trondheim</t>
+          <t>Oslo/Bi</t>
         </is>
       </c>
       <c r="R218" s="16" t="n">
-        <v>12.08</v>
+        <v>13.07</v>
       </c>
       <c r="T218" s="5" t="n"/>
     </row>
     <row r="219" ht="13" customHeight="1">
       <c r="B219" s="14" t="inlineStr">
         <is>
-          <t>3000m</t>
+          <t>100m</t>
         </is>
       </c>
       <c r="C219" s="7" t="inlineStr">
         <is>
-          <t>Per-Christian Myrnes Pedersen</t>
+          <t>Oliver Tomala</t>
         </is>
       </c>
       <c r="D219" s="7" t="n">
-        <v>1986</v>
-      </c>
-      <c r="E219" s="17" t="inlineStr">
-        <is>
-          <t>9,08,98</t>
-        </is>
+        <v>2007</v>
+      </c>
+      <c r="E219" s="15" t="n">
+        <v>11.64</v>
       </c>
       <c r="F219" s="7" t="n">
-        <v>655</v>
+        <v>688</v>
       </c>
       <c r="G219" s="7" t="inlineStr">
         <is>
-          <t>Harstad</t>
+          <t>Trondheim</t>
         </is>
       </c>
       <c r="H219" s="16" t="n">
-        <v>11.09</v>
+        <v>12.08</v>
       </c>
       <c r="J219" s="5" t="n"/>
       <c r="L219" s="14" t="inlineStr">
         <is>
-          <t>100m</t>
+          <t>3000m</t>
         </is>
       </c>
       <c r="M219" s="7" t="inlineStr">
         <is>
-          <t>Simen Johan Teigstad</t>
+          <t>Per-Christian Myrnes Pedersen</t>
         </is>
       </c>
       <c r="N219" s="7" t="n">
-        <v>2005</v>
-      </c>
-      <c r="O219" s="15" t="n">
-        <v>11.91</v>
+        <v>1986</v>
+      </c>
+      <c r="O219" s="17" t="inlineStr">
+        <is>
+          <t>9,08,98</t>
+        </is>
       </c>
       <c r="P219" s="7" t="n">
-        <v>629</v>
+        <v>655</v>
       </c>
       <c r="Q219" s="7" t="inlineStr">
         <is>
-          <t>Seinäjoki/FIN</t>
+          <t>Harstad</t>
         </is>
       </c>
       <c r="R219" s="16" t="n">
-        <v>11.06</v>
+        <v>11.09</v>
       </c>
       <c r="T219" s="5" t="n"/>
     </row>
     <row r="220" ht="13" customHeight="1">
       <c r="B220" s="14" t="inlineStr">
         <is>
-          <t>400m</t>
+          <t>Lengde</t>
         </is>
       </c>
       <c r="C220" s="7" t="inlineStr">
         <is>
-          <t>Birk Arvola</t>
+          <t>Sondre Witzøe</t>
         </is>
       </c>
       <c r="D220" s="7" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="E220" s="15" t="n">
-        <v>53.13</v>
+        <v>6.21</v>
       </c>
       <c r="F220" s="7" t="n">
-        <v>639</v>
+        <v>654</v>
       </c>
       <c r="G220" s="7" t="inlineStr">
         <is>
-          <t>Sortland</t>
+          <t>Bærum</t>
         </is>
       </c>
       <c r="H220" s="16" t="n">
-        <v>20.08</v>
+        <v>12.02</v>
       </c>
       <c r="J220" s="5" t="n"/>
       <c r="L220" s="14" t="inlineStr">
         <is>
-          <t>Stav</t>
+          <t>400m</t>
         </is>
       </c>
       <c r="M220" s="7" t="inlineStr">
         <is>
-          <t>Siver Olavsbråten Ebbestad</t>
+          <t>Birk Arvola</t>
         </is>
       </c>
       <c r="N220" s="7" t="n">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="O220" s="15" t="n">
-        <v>3.54</v>
+        <v>53.13</v>
       </c>
       <c r="P220" s="7" t="n">
-        <v>623</v>
+        <v>639</v>
       </c>
       <c r="Q220" s="7" t="inlineStr">
         <is>
-          <t>Gøteborg/SWE</t>
+          <t>Sortland</t>
         </is>
       </c>
       <c r="R220" s="16" t="n">
-        <v>18.06</v>
+        <v>20.08</v>
       </c>
       <c r="T220" s="5" t="n"/>
     </row>
     <row r="221" ht="13" customHeight="1">
       <c r="B221" s="14" t="inlineStr">
         <is>
-          <t>3000m</t>
+          <t>Stav</t>
         </is>
       </c>
       <c r="C221" s="7" t="inlineStr">
         <is>
-          <t>Erik Fossen Nilsen</t>
+          <t>Siver Olavsbråten Ebbestad</t>
         </is>
       </c>
       <c r="D221" s="7" t="n">
-        <v>1987</v>
-      </c>
-      <c r="E221" s="17" t="inlineStr">
-        <is>
-          <t>9,17,89</t>
-        </is>
+        <v>2008</v>
+      </c>
+      <c r="E221" s="15" t="n">
+        <v>3.54</v>
       </c>
       <c r="F221" s="7" t="n">
         <v>623</v>
       </c>
       <c r="G221" s="7" t="inlineStr">
         <is>
-          <t>Narvik</t>
+          <t>Gøteborg/SWE</t>
         </is>
       </c>
       <c r="H221" s="16" t="n">
-        <v>11.06</v>
+        <v>18.06</v>
       </c>
       <c r="J221" s="5" t="n"/>
       <c r="L221" s="14" t="inlineStr">
         <is>
-          <t>100m</t>
+          <t>3000m</t>
         </is>
       </c>
       <c r="M221" s="7" t="inlineStr">
         <is>
-          <t>Sander Skarre Lindseth</t>
+          <t>Erik Fossen Nilsen</t>
         </is>
       </c>
       <c r="N221" s="7" t="n">
-        <v>2006</v>
-      </c>
-      <c r="O221" s="15" t="n">
-        <v>11.96</v>
+        <v>1987</v>
+      </c>
+      <c r="O221" s="17" t="inlineStr">
+        <is>
+          <t>9,17,89</t>
+        </is>
       </c>
       <c r="P221" s="7" t="n">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="Q221" s="7" t="inlineStr">
         <is>
-          <t>Sande</t>
+          <t>Narvik</t>
         </is>
       </c>
       <c r="R221" s="16" t="n">
-        <v>16.05</v>
+        <v>11.06</v>
       </c>
       <c r="T221" s="5" t="n"/>
     </row>
     <row r="222" ht="13" customHeight="1">
       <c r="B222" s="14" t="inlineStr">
         <is>
-          <t>400m</t>
+          <t>100m</t>
         </is>
       </c>
       <c r="C222" s="7" t="inlineStr">
         <is>
-          <t>Oskar Stattin</t>
+          <t>Sander Skarre Lindseth</t>
         </is>
       </c>
       <c r="D222" s="7" t="n">
         <v>2006</v>
       </c>
       <c r="E222" s="15" t="n">
-        <v>53.72</v>
+        <v>11.96</v>
       </c>
       <c r="F222" s="7" t="n">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="G222" s="7" t="inlineStr">
         <is>
-          <t>Harstad</t>
+          <t>Sande</t>
         </is>
       </c>
       <c r="H222" s="16" t="n">
-        <v>7.06</v>
+        <v>16.05</v>
       </c>
       <c r="J222" s="5" t="n"/>
       <c r="L222" s="14" t="inlineStr">
         <is>
-          <t>100m</t>
+          <t>400m</t>
         </is>
       </c>
       <c r="M222" s="7" t="inlineStr">
         <is>
-          <t>Alexander Tomala</t>
+          <t>Oskar Stattin</t>
         </is>
       </c>
       <c r="N222" s="7" t="n">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="O222" s="15" t="n">
-        <v>11.99</v>
+        <v>53.72</v>
       </c>
       <c r="P222" s="7" t="n">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="Q222" s="7" t="inlineStr">
         <is>
-          <t>Trondheim</t>
+          <t>Harstad</t>
         </is>
       </c>
       <c r="R222" s="16" t="n">
-        <v>12.08</v>
+        <v>7.06</v>
       </c>
       <c r="T222" s="5" t="n"/>
     </row>
     <row r="223" ht="13" customHeight="1">
       <c r="B223" s="14" t="inlineStr">
         <is>
-          <t>800m</t>
+          <t>100m</t>
         </is>
       </c>
       <c r="C223" s="7" t="inlineStr">
         <is>
-          <t>Stian Markussen Eilertsen</t>
+          <t>Alexander Tomala</t>
         </is>
       </c>
       <c r="D223" s="7" t="n">
-        <v>1986</v>
-      </c>
-      <c r="E223" s="17" t="inlineStr">
-        <is>
-          <t>2,04,45</t>
-        </is>
+        <v>2005</v>
+      </c>
+      <c r="E223" s="15" t="n">
+        <v>11.99</v>
       </c>
       <c r="F223" s="7" t="n">
-        <v>607</v>
+        <v>613</v>
       </c>
       <c r="G223" s="7" t="inlineStr">
         <is>
-          <t>Narvik</t>
+          <t>Trondheim</t>
         </is>
       </c>
       <c r="H223" s="16" t="n">
-        <v>12.06</v>
+        <v>12.08</v>
       </c>
       <c r="J223" s="5" t="n"/>
       <c r="L223" s="14" t="inlineStr">
         <is>
-          <t>60m</t>
+          <t>800m</t>
         </is>
       </c>
       <c r="M223" s="7" t="inlineStr">
         <is>
-          <t>Sander Skarre Lindseth</t>
+          <t>Stian Markussen Eilertsen</t>
         </is>
       </c>
       <c r="N223" s="7" t="n">
-        <v>2006</v>
-      </c>
-      <c r="O223" s="15" t="n">
-        <v>7.65</v>
+        <v>1986</v>
+      </c>
+      <c r="O223" s="17" t="inlineStr">
+        <is>
+          <t>2,04,45</t>
+        </is>
       </c>
       <c r="P223" s="7" t="n">
         <v>607</v>
       </c>
       <c r="Q223" s="7" t="inlineStr">
         <is>
-          <t>Grimstad</t>
+          <t>Narvik</t>
         </is>
       </c>
       <c r="R223" s="16" t="n">
-        <v>13.03</v>
+        <v>12.06</v>
       </c>
       <c r="T223" s="5" t="n"/>
     </row>
     <row r="224" ht="13" customHeight="1">
       <c r="B224" s="14" t="inlineStr">
         <is>
-          <t>Lengde</t>
+          <t>60m</t>
         </is>
       </c>
       <c r="C224" s="7" t="inlineStr">
         <is>
-          <t>Oskar Stattin</t>
+          <t>Sander Skarre Lindseth</t>
         </is>
       </c>
       <c r="D224" s="7" t="n">
         <v>2006</v>
       </c>
       <c r="E224" s="15" t="n">
-        <v>5.87</v>
+        <v>7.65</v>
       </c>
       <c r="F224" s="7" t="n">
-        <v>577</v>
+        <v>607</v>
       </c>
       <c r="G224" s="7" t="inlineStr">
         <is>
-          <t>Harstad</t>
+          <t>Grimstad</t>
         </is>
       </c>
       <c r="H224" s="16" t="n">
-        <v>24.05</v>
+        <v>13.03</v>
       </c>
       <c r="J224" s="5" t="n"/>
       <c r="L224" s="14" t="inlineStr">
         <is>
-          <t>400m</t>
+          <t>Lengde</t>
         </is>
       </c>
       <c r="M224" s="7" t="inlineStr">
         <is>
-          <t>Oliver Tomala</t>
+          <t>Oskar Stattin</t>
         </is>
       </c>
       <c r="N224" s="7" t="n">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="O224" s="15" t="n">
-        <v>54.01</v>
+        <v>5.87</v>
       </c>
       <c r="P224" s="7" t="n">
-        <v>603</v>
+        <v>577</v>
       </c>
       <c r="Q224" s="7" t="inlineStr">
         <is>
-          <t>Geithus</t>
+          <t>Harstad</t>
         </is>
       </c>
       <c r="R224" s="16" t="n">
-        <v>11.09</v>
+        <v>24.05</v>
       </c>
       <c r="T224" s="5" t="n"/>
     </row>
     <row r="225" ht="13" customHeight="1">
       <c r="B225" s="14" t="inlineStr">
         <is>
-          <t>Lengde</t>
+          <t>400m</t>
         </is>
       </c>
       <c r="C225" s="7" t="inlineStr">
         <is>
-          <t>Kristian Sheath</t>
+          <t>Oliver Tomala</t>
         </is>
       </c>
       <c r="D225" s="7" t="n">
-        <v>2005</v>
+        <v>2007</v>
       </c>
       <c r="E225" s="15" t="n">
-        <v>5.64</v>
+        <v>54.01</v>
       </c>
       <c r="F225" s="7" t="n">
-        <v>523</v>
+        <v>603</v>
       </c>
       <c r="G225" s="7" t="inlineStr">
         <is>
-          <t>Harstad</t>
+          <t>Geithus</t>
         </is>
       </c>
       <c r="H225" s="16" t="n">
@@ -26424,83 +26426,83 @@
       </c>
       <c r="M225" s="7" t="inlineStr">
         <is>
-          <t>Sander Skarre Lindseth</t>
+          <t>Kristian Sheath</t>
         </is>
       </c>
       <c r="N225" s="7" t="n">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="O225" s="15" t="n">
-        <v>5.7</v>
+        <v>5.64</v>
       </c>
       <c r="P225" s="7" t="n">
-        <v>537</v>
+        <v>523</v>
       </c>
       <c r="Q225" s="7" t="inlineStr">
         <is>
-          <t>Sande</t>
+          <t>Harstad</t>
         </is>
       </c>
       <c r="R225" s="16" t="n">
-        <v>16.05</v>
+        <v>11.09</v>
       </c>
       <c r="T225" s="5" t="n"/>
     </row>
     <row r="226" ht="13" customHeight="1">
       <c r="B226" s="14" t="inlineStr">
         <is>
-          <t>Tresteg</t>
+          <t>Lengde</t>
         </is>
       </c>
       <c r="C226" s="7" t="inlineStr">
         <is>
-          <t>Oskar Stattin</t>
+          <t>Sander Skarre Lindseth</t>
         </is>
       </c>
       <c r="D226" s="7" t="n">
         <v>2006</v>
       </c>
       <c r="E226" s="15" t="n">
-        <v>11.56</v>
+        <v>5.7</v>
       </c>
       <c r="F226" s="7" t="n">
-        <v>511</v>
+        <v>537</v>
       </c>
       <c r="G226" s="7" t="inlineStr">
         <is>
-          <t>Steinkjer</t>
+          <t>Sande</t>
         </is>
       </c>
       <c r="H226" s="16" t="n">
-        <v>4.03</v>
+        <v>16.05</v>
       </c>
       <c r="J226" s="5" t="n"/>
       <c r="L226" s="14" t="inlineStr">
         <is>
-          <t>Høyde</t>
+          <t>Tresteg</t>
         </is>
       </c>
       <c r="M226" s="7" t="inlineStr">
         <is>
-          <t>Lucas Bricot</t>
+          <t>Oskar Stattin</t>
         </is>
       </c>
       <c r="N226" s="7" t="n">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="O226" s="15" t="n">
-        <v>1.65</v>
+        <v>11.56</v>
       </c>
       <c r="P226" s="7" t="n">
         <v>511</v>
       </c>
       <c r="Q226" s="7" t="inlineStr">
         <is>
-          <t>Drammen</t>
+          <t>Steinkjer</t>
         </is>
       </c>
       <c r="R226" s="16" t="n">
-        <v>7.05</v>
+        <v>4.03</v>
       </c>
       <c r="T226" s="5" t="n"/>
     </row>
@@ -26512,53 +26514,53 @@
       </c>
       <c r="C227" s="7" t="inlineStr">
         <is>
-          <t>Leif-Andreas Borgersen</t>
+          <t>Lucas Bricot</t>
         </is>
       </c>
       <c r="D227" s="7" t="n">
         <v>2008</v>
       </c>
       <c r="E227" s="15" t="n">
-        <v>1.55</v>
+        <v>1.65</v>
       </c>
       <c r="F227" s="7" t="n">
-        <v>408</v>
+        <v>511</v>
       </c>
       <c r="G227" s="7" t="inlineStr">
         <is>
-          <t>Finnsnes</t>
+          <t>Drammen</t>
         </is>
       </c>
       <c r="H227" s="16" t="n">
-        <v>4.06</v>
+        <v>7.05</v>
       </c>
       <c r="J227" s="5" t="n"/>
       <c r="L227" s="14" t="inlineStr">
         <is>
-          <t>Stav</t>
+          <t>Høyde</t>
         </is>
       </c>
       <c r="M227" s="7" t="inlineStr">
         <is>
-          <t>Tobias Kalmo Thorbjørnsen</t>
+          <t>Leif-Andreas Borgersen</t>
         </is>
       </c>
       <c r="N227" s="7" t="n">
-        <v>2006</v>
+        <v>2008</v>
       </c>
       <c r="O227" s="15" t="n">
-        <v>3</v>
+        <v>1.55</v>
       </c>
       <c r="P227" s="7" t="n">
-        <v>500</v>
+        <v>408</v>
       </c>
       <c r="Q227" s="7" t="inlineStr">
         <is>
-          <t>Hamar</t>
+          <t>Finnsnes</t>
         </is>
       </c>
       <c r="R227" s="16" t="n">
-        <v>22.05</v>
+        <v>4.06</v>
       </c>
       <c r="T227" s="5" t="n"/>
     </row>
@@ -26595,7 +26597,7 @@
         </is>
       </c>
       <c r="F229" s="20" t="n">
-        <v>7173</v>
+        <v>7637</v>
       </c>
       <c r="J229" s="5" t="n"/>
       <c r="L229" s="19" t="inlineStr">
@@ -26612,7 +26614,7 @@
         </is>
       </c>
       <c r="P229" s="20" t="n">
-        <v>7387</v>
+        <v>7173</v>
       </c>
       <c r="T229" s="5" t="n"/>
     </row>
@@ -26635,7 +26637,7 @@
         </is>
       </c>
       <c r="F231" s="20" t="n">
-        <v>15493</v>
+        <v>15724</v>
       </c>
       <c r="J231" s="5" t="n"/>
       <c r="L231" s="19" t="inlineStr">
@@ -26652,7 +26654,7 @@
         </is>
       </c>
       <c r="P231" s="20" t="n">
-        <v>15250</v>
+        <v>15493</v>
       </c>
       <c r="T231" s="5" t="n"/>
     </row>
@@ -27046,11 +27048,11 @@
       </c>
       <c r="Q246" s="7" t="inlineStr">
         <is>
-          <t>Leikvang</t>
+          <t>Arna</t>
         </is>
       </c>
       <c r="R246" s="16" t="n">
-        <v>11.09</v>
+        <v>21.09</v>
       </c>
       <c r="T246" s="5" t="n"/>
     </row>
@@ -27877,30 +27879,30 @@
       <c r="J264" s="5" t="n"/>
       <c r="L264" s="14" t="inlineStr">
         <is>
-          <t>Diskos</t>
+          <t>60m</t>
         </is>
       </c>
       <c r="M264" s="7" t="inlineStr">
         <is>
-          <t>Stein Fossen</t>
+          <t>Morten Solheim</t>
         </is>
       </c>
       <c r="N264" s="7" t="n">
-        <v>1968</v>
+        <v>1976</v>
       </c>
       <c r="O264" s="15" t="n">
-        <v>28.92</v>
+        <v>7.94</v>
       </c>
       <c r="P264" s="7" t="n">
-        <v>452</v>
+        <v>514</v>
       </c>
       <c r="Q264" s="7" t="inlineStr">
         <is>
-          <t>Knarvik</t>
+          <t>Arna</t>
         </is>
       </c>
       <c r="R264" s="16" t="n">
-        <v>21.06</v>
+        <v>21.09</v>
       </c>
       <c r="T264" s="5" t="n"/>
     </row>
@@ -27937,30 +27939,30 @@
       <c r="J265" s="5" t="n"/>
       <c r="L265" s="14" t="inlineStr">
         <is>
-          <t>100m</t>
+          <t>Diskos</t>
         </is>
       </c>
       <c r="M265" s="7" t="inlineStr">
         <is>
-          <t>Morten Solheim</t>
+          <t>Stein Fossen</t>
         </is>
       </c>
       <c r="N265" s="7" t="n">
-        <v>1976</v>
+        <v>1968</v>
       </c>
       <c r="O265" s="15" t="n">
-        <v>12.83</v>
+        <v>28.92</v>
       </c>
       <c r="P265" s="7" t="n">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="Q265" s="7" t="inlineStr">
         <is>
-          <t>Ravnanger</t>
+          <t>Knarvik</t>
         </is>
       </c>
       <c r="R265" s="16" t="n">
-        <v>24.08</v>
+        <v>21.06</v>
       </c>
       <c r="T265" s="5" t="n"/>
     </row>
@@ -27997,32 +27999,30 @@
       <c r="J266" s="5" t="n"/>
       <c r="L266" s="14" t="inlineStr">
         <is>
-          <t>5000m</t>
+          <t>100m</t>
         </is>
       </c>
       <c r="M266" s="7" t="inlineStr">
         <is>
-          <t>Christer Sælen</t>
+          <t>Morten Solheim</t>
         </is>
       </c>
       <c r="N266" s="7" t="n">
-        <v>1981</v>
-      </c>
-      <c r="O266" s="17" t="inlineStr">
-        <is>
-          <t>18,24,97</t>
-        </is>
+        <v>1976</v>
+      </c>
+      <c r="O266" s="15" t="n">
+        <v>12.83</v>
       </c>
       <c r="P266" s="7" t="n">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="Q266" s="7" t="inlineStr">
         <is>
-          <t>Arna</t>
+          <t>Ravnanger</t>
         </is>
       </c>
       <c r="R266" s="16" t="n">
-        <v>15.08</v>
+        <v>24.08</v>
       </c>
       <c r="T266" s="5" t="n"/>
     </row>
@@ -28059,22 +28059,24 @@
       <c r="J267" s="5" t="n"/>
       <c r="L267" s="14" t="inlineStr">
         <is>
-          <t>Høyde u.t</t>
+          <t>5000m</t>
         </is>
       </c>
       <c r="M267" s="7" t="inlineStr">
         <is>
-          <t>Oddvin Årdalsbakke</t>
+          <t>Christer Sælen</t>
         </is>
       </c>
       <c r="N267" s="7" t="n">
-        <v>1962</v>
-      </c>
-      <c r="O267" s="15" t="n">
-        <v>1.27</v>
+        <v>1981</v>
+      </c>
+      <c r="O267" s="17" t="inlineStr">
+        <is>
+          <t>18,24,97</t>
+        </is>
       </c>
       <c r="P267" s="7" t="n">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="Q267" s="7" t="inlineStr">
         <is>
@@ -28082,7 +28084,7 @@
         </is>
       </c>
       <c r="R267" s="16" t="n">
-        <v>14.03</v>
+        <v>15.08</v>
       </c>
       <c r="T267" s="5" t="n"/>
     </row>
@@ -28119,32 +28121,30 @@
       <c r="J268" s="5" t="n"/>
       <c r="L268" s="14" t="inlineStr">
         <is>
-          <t>3000m</t>
+          <t>Høyde u.t</t>
         </is>
       </c>
       <c r="M268" s="7" t="inlineStr">
         <is>
-          <t>Nils Tore Sæterdal</t>
+          <t>Oddvin Årdalsbakke</t>
         </is>
       </c>
       <c r="N268" s="7" t="n">
-        <v>1967</v>
-      </c>
-      <c r="O268" s="17" t="inlineStr">
-        <is>
-          <t>10,40,22</t>
-        </is>
+        <v>1962</v>
+      </c>
+      <c r="O268" s="15" t="n">
+        <v>1.27</v>
       </c>
       <c r="P268" s="7" t="n">
-        <v>381</v>
+        <v>398</v>
       </c>
       <c r="Q268" s="7" t="inlineStr">
         <is>
-          <t>Osterøy</t>
+          <t>Arna</t>
         </is>
       </c>
       <c r="R268" s="16" t="n">
-        <v>22.08</v>
+        <v>14.03</v>
       </c>
       <c r="T268" s="5" t="n"/>
     </row>
@@ -28181,30 +28181,32 @@
       <c r="J269" s="5" t="n"/>
       <c r="L269" s="14" t="inlineStr">
         <is>
-          <t>Lengde u.t</t>
+          <t>3000m</t>
         </is>
       </c>
       <c r="M269" s="7" t="inlineStr">
         <is>
-          <t>Oddvin Årdalsbakke</t>
+          <t>Nils Tore Sæterdal</t>
         </is>
       </c>
       <c r="N269" s="7" t="n">
-        <v>1962</v>
-      </c>
-      <c r="O269" s="15" t="n">
-        <v>2.51</v>
+        <v>1967</v>
+      </c>
+      <c r="O269" s="17" t="inlineStr">
+        <is>
+          <t>10,40,22</t>
+        </is>
       </c>
       <c r="P269" s="7" t="n">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="Q269" s="7" t="inlineStr">
         <is>
-          <t>Arna</t>
+          <t>Osterøy</t>
         </is>
       </c>
       <c r="R269" s="16" t="n">
-        <v>14.03</v>
+        <v>22.08</v>
       </c>
       <c r="T269" s="5" t="n"/>
     </row>
@@ -28299,32 +28301,30 @@
       <c r="J271" s="5" t="n"/>
       <c r="L271" s="14" t="inlineStr">
         <is>
-          <t>3000m</t>
+          <t>Lengde u.t</t>
         </is>
       </c>
       <c r="M271" s="7" t="inlineStr">
         <is>
-          <t>Espen Irgens Haugen</t>
+          <t>Oddvin Årdalsbakke</t>
         </is>
       </c>
       <c r="N271" s="7" t="n">
-        <v>1985</v>
-      </c>
-      <c r="O271" s="17" t="inlineStr">
-        <is>
-          <t>10,43,35</t>
-        </is>
+        <v>1962</v>
+      </c>
+      <c r="O271" s="15" t="n">
+        <v>2.51</v>
       </c>
       <c r="P271" s="7" t="n">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="Q271" s="7" t="inlineStr">
         <is>
-          <t>Osterøy</t>
+          <t>Arna</t>
         </is>
       </c>
       <c r="R271" s="16" t="n">
-        <v>22.08</v>
+        <v>14.03</v>
       </c>
       <c r="T271" s="5" t="n"/>
     </row>
@@ -28339,32 +28339,32 @@
       <c r="J272" s="5" t="n"/>
       <c r="L272" s="14" t="inlineStr">
         <is>
-          <t>1500m</t>
+          <t>3000m</t>
         </is>
       </c>
       <c r="M272" s="7" t="inlineStr">
         <is>
-          <t>Nils Tore Sæterdal</t>
+          <t>Espen Irgens Haugen</t>
         </is>
       </c>
       <c r="N272" s="7" t="n">
-        <v>1967</v>
+        <v>1985</v>
       </c>
       <c r="O272" s="17" t="inlineStr">
         <is>
-          <t>4,56,18</t>
+          <t>10,43,35</t>
         </is>
       </c>
       <c r="P272" s="7" t="n">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="Q272" s="7" t="inlineStr">
         <is>
-          <t>Arna</t>
+          <t>Osterøy</t>
         </is>
       </c>
       <c r="R272" s="16" t="n">
-        <v>15.08</v>
+        <v>22.08</v>
       </c>
       <c r="T272" s="5" t="n"/>
     </row>
@@ -28379,24 +28379,24 @@
       <c r="J273" s="5" t="n"/>
       <c r="L273" s="14" t="inlineStr">
         <is>
-          <t>800m</t>
+          <t>1500m</t>
         </is>
       </c>
       <c r="M273" s="7" t="inlineStr">
         <is>
-          <t>Christer Sælen</t>
+          <t>Nils Tore Sæterdal</t>
         </is>
       </c>
       <c r="N273" s="7" t="n">
-        <v>1981</v>
+        <v>1967</v>
       </c>
       <c r="O273" s="17" t="inlineStr">
         <is>
-          <t>2,24,12</t>
+          <t>4,56,18</t>
         </is>
       </c>
       <c r="P273" s="7" t="n">
-        <v>355</v>
+        <v>372</v>
       </c>
       <c r="Q273" s="7" t="inlineStr">
         <is>
@@ -28404,7 +28404,7 @@
         </is>
       </c>
       <c r="R273" s="16" t="n">
-        <v>6.07</v>
+        <v>15.08</v>
       </c>
       <c r="T273" s="5" t="n"/>
     </row>
@@ -28419,32 +28419,32 @@
       <c r="J274" s="5" t="n"/>
       <c r="L274" s="14" t="inlineStr">
         <is>
-          <t>3000m</t>
+          <t>800m</t>
         </is>
       </c>
       <c r="M274" s="7" t="inlineStr">
         <is>
-          <t>Lars Olav Brattabø</t>
+          <t>Christer Sælen</t>
         </is>
       </c>
       <c r="N274" s="7" t="n">
-        <v>1973</v>
+        <v>1981</v>
       </c>
       <c r="O274" s="17" t="inlineStr">
         <is>
-          <t>10,55,67</t>
+          <t>2,24,12</t>
         </is>
       </c>
       <c r="P274" s="7" t="n">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="Q274" s="7" t="inlineStr">
         <is>
-          <t>Osterøy</t>
+          <t>Arna</t>
         </is>
       </c>
       <c r="R274" s="16" t="n">
-        <v>2.06</v>
+        <v>6.07</v>
       </c>
       <c r="T274" s="5" t="n"/>
     </row>
@@ -28498,7 +28498,7 @@
         </is>
       </c>
       <c r="P276" s="20" t="n">
-        <v>4869</v>
+        <v>5039</v>
       </c>
       <c r="T276" s="5" t="n"/>
     </row>
@@ -28538,7 +28538,7 @@
         </is>
       </c>
       <c r="P278" s="20" t="n">
-        <v>13541</v>
+        <v>13711</v>
       </c>
       <c r="T278" s="5" t="n"/>
     </row>
@@ -28562,7 +28562,7 @@
         </is>
       </c>
       <c r="M280" s="20" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T280" s="5" t="n"/>
     </row>
@@ -30658,7 +30658,7 @@
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>23266</v>
+        <v>23320</v>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
@@ -30850,11 +30850,11 @@
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>(28/13)</t>
+          <t>(29/14)</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>18409</v>
+        <v>18836</v>
       </c>
       <c r="E13" s="4" t="inlineStr">
         <is>
@@ -33023,11 +33023,11 @@
       </c>
       <c r="M43" s="7" t="inlineStr">
         <is>
-          <t>Andrea Igeltjørn Lyngholm</t>
+          <t>Eline Soma</t>
         </is>
       </c>
       <c r="N43" s="7" t="n">
-        <v>2005</v>
+        <v>2007</v>
       </c>
       <c r="O43" s="15" t="n">
         <v>1.55</v>
@@ -33041,7 +33041,7 @@
         </is>
       </c>
       <c r="R43" s="16" t="n">
-        <v>27.02</v>
+        <v>25.08</v>
       </c>
       <c r="T43" s="5" t="n"/>
     </row>
@@ -33081,11 +33081,11 @@
       </c>
       <c r="M44" s="7" t="inlineStr">
         <is>
-          <t>Eline Soma</t>
+          <t>Andrea Igeltjørn Lyngholm</t>
         </is>
       </c>
       <c r="N44" s="7" t="n">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="O44" s="15" t="n">
         <v>1.55</v>
@@ -33099,7 +33099,7 @@
         </is>
       </c>
       <c r="R44" s="16" t="n">
-        <v>25.08</v>
+        <v>27.02</v>
       </c>
       <c r="T44" s="5" t="n"/>
     </row>
@@ -34542,30 +34542,30 @@
       <c r="J83" s="5" t="n"/>
       <c r="L83" s="14" t="inlineStr">
         <is>
-          <t>100m</t>
+          <t>Diskos</t>
         </is>
       </c>
       <c r="M83" s="7" t="inlineStr">
         <is>
-          <t>Martine Hjørnevik</t>
+          <t>Helene Ramslien</t>
         </is>
       </c>
       <c r="N83" s="7" t="n">
-        <v>2001</v>
+        <v>2006</v>
       </c>
       <c r="O83" s="15" t="n">
-        <v>12.38</v>
+        <v>45.9</v>
       </c>
       <c r="P83" s="7" t="n">
-        <v>781</v>
+        <v>806</v>
       </c>
       <c r="Q83" s="7" t="inlineStr">
         <is>
-          <t>Jessheim</t>
+          <t>Knarvik</t>
         </is>
       </c>
       <c r="R83" s="16" t="n">
-        <v>7.08</v>
+        <v>18.09</v>
       </c>
       <c r="T83" s="5" t="n"/>
     </row>
@@ -34600,30 +34600,30 @@
       <c r="J84" s="5" t="n"/>
       <c r="L84" s="14" t="inlineStr">
         <is>
-          <t>Diskos</t>
+          <t>100m</t>
         </is>
       </c>
       <c r="M84" s="7" t="inlineStr">
         <is>
-          <t>Helene Ramslien</t>
+          <t>Martine Hjørnevik</t>
         </is>
       </c>
       <c r="N84" s="7" t="n">
-        <v>2006</v>
+        <v>2001</v>
       </c>
       <c r="O84" s="15" t="n">
-        <v>44.05</v>
+        <v>12.38</v>
       </c>
       <c r="P84" s="7" t="n">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="Q84" s="7" t="inlineStr">
         <is>
-          <t>Gloppen</t>
+          <t>Jessheim</t>
         </is>
       </c>
       <c r="R84" s="16" t="n">
-        <v>11.09</v>
+        <v>7.08</v>
       </c>
       <c r="T84" s="5" t="n"/>
     </row>
@@ -35130,32 +35130,30 @@
       <c r="J93" s="5" t="n"/>
       <c r="L93" s="14" t="inlineStr">
         <is>
-          <t>800m</t>
+          <t>Lengde u.t</t>
         </is>
       </c>
       <c r="M93" s="7" t="inlineStr">
         <is>
-          <t>Alexandra Tunes Lund</t>
+          <t>Julie Dicko Erichsen</t>
         </is>
       </c>
       <c r="N93" s="7" t="n">
-        <v>2007</v>
-      </c>
-      <c r="O93" s="17" t="inlineStr">
-        <is>
-          <t>2,19,99</t>
-        </is>
+        <v>2001</v>
+      </c>
+      <c r="O93" s="15" t="n">
+        <v>2.58</v>
       </c>
       <c r="P93" s="7" t="n">
-        <v>667</v>
+        <v>678</v>
       </c>
       <c r="Q93" s="7" t="inlineStr">
         <is>
-          <t>Rosendal</t>
+          <t>Leikvang</t>
         </is>
       </c>
       <c r="R93" s="16" t="n">
-        <v>4.06</v>
+        <v>28.09</v>
       </c>
       <c r="T93" s="5" t="n"/>
     </row>
@@ -35190,30 +35188,32 @@
       <c r="J94" s="5" t="n"/>
       <c r="L94" s="14" t="inlineStr">
         <is>
-          <t>200m</t>
+          <t>800m</t>
         </is>
       </c>
       <c r="M94" s="7" t="inlineStr">
         <is>
-          <t>Nathalie Svanevik Hølleland</t>
+          <t>Alexandra Tunes Lund</t>
         </is>
       </c>
       <c r="N94" s="7" t="n">
         <v>2007</v>
       </c>
-      <c r="O94" s="15" t="n">
-        <v>26.83</v>
+      <c r="O94" s="17" t="inlineStr">
+        <is>
+          <t>2,19,99</t>
+        </is>
       </c>
       <c r="P94" s="7" t="n">
-        <v>662</v>
+        <v>667</v>
       </c>
       <c r="Q94" s="7" t="inlineStr">
         <is>
-          <t>Steinkjer</t>
+          <t>Rosendal</t>
         </is>
       </c>
       <c r="R94" s="16" t="n">
-        <v>6.03</v>
+        <v>4.06</v>
       </c>
       <c r="T94" s="5" t="n"/>
     </row>
@@ -35248,30 +35248,30 @@
       <c r="J95" s="5" t="n"/>
       <c r="L95" s="14" t="inlineStr">
         <is>
-          <t>Slegge</t>
+          <t>200m</t>
         </is>
       </c>
       <c r="M95" s="7" t="inlineStr">
         <is>
-          <t>Stina Leivestad Morvik</t>
+          <t>Nathalie Svanevik Hølleland</t>
         </is>
       </c>
       <c r="N95" s="7" t="n">
-        <v>2004</v>
+        <v>2007</v>
       </c>
       <c r="O95" s="15" t="n">
-        <v>38.11</v>
+        <v>26.83</v>
       </c>
       <c r="P95" s="7" t="n">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="Q95" s="7" t="inlineStr">
         <is>
-          <t>Knarvik</t>
+          <t>Steinkjer</t>
         </is>
       </c>
       <c r="R95" s="16" t="n">
-        <v>26.03</v>
+        <v>6.03</v>
       </c>
       <c r="T95" s="5" t="n"/>
     </row>
@@ -35311,25 +35311,25 @@
       </c>
       <c r="M96" s="7" t="inlineStr">
         <is>
-          <t>Ida Ramslien</t>
+          <t>Stina Leivestad Morvik</t>
         </is>
       </c>
       <c r="N96" s="7" t="n">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="O96" s="15" t="n">
-        <v>37.56</v>
+        <v>38.17</v>
       </c>
       <c r="P96" s="7" t="n">
-        <v>651</v>
+        <v>659</v>
       </c>
       <c r="Q96" s="7" t="inlineStr">
         <is>
-          <t>Bergen</t>
+          <t>Knarvik</t>
         </is>
       </c>
       <c r="R96" s="16" t="n">
-        <v>12.07</v>
+        <v>18.09</v>
       </c>
       <c r="T96" s="5" t="n"/>
     </row>
@@ -35383,7 +35383,7 @@
         </is>
       </c>
       <c r="P98" s="20" t="n">
-        <v>10717</v>
+        <v>10771</v>
       </c>
       <c r="T98" s="5" t="n"/>
     </row>
@@ -35423,7 +35423,7 @@
         </is>
       </c>
       <c r="P100" s="20" t="n">
-        <v>23266</v>
+        <v>23320</v>
       </c>
       <c r="T100" s="5" t="n"/>
     </row>
@@ -39695,11 +39695,11 @@
       </c>
       <c r="G199" s="7" t="inlineStr">
         <is>
-          <t>Oslo/Bi</t>
+          <t>Oslo/St</t>
         </is>
       </c>
       <c r="H199" s="16" t="n">
-        <v>28.05</v>
+        <v>11.09</v>
       </c>
       <c r="J199" s="5" t="n"/>
       <c r="L199" s="14" t="inlineStr">
@@ -40773,25 +40773,25 @@
       </c>
       <c r="C228" s="7" t="inlineStr">
         <is>
-          <t>Maria Døske</t>
+          <t>Hanna Haugsvær</t>
         </is>
       </c>
       <c r="D228" s="7" t="n">
         <v>2005</v>
       </c>
       <c r="E228" s="15" t="n">
-        <v>11.59</v>
+        <v>11.58</v>
       </c>
       <c r="F228" s="7" t="n">
         <v>691</v>
       </c>
       <c r="G228" s="7" t="inlineStr">
         <is>
-          <t>Bærum</t>
+          <t>Ulsteinvik</t>
         </is>
       </c>
       <c r="H228" s="16" t="n">
-        <v>26.08</v>
+        <v>5.02</v>
       </c>
       <c r="J228" s="5" t="n"/>
       <c r="L228" s="14" t="inlineStr">
@@ -41455,25 +41455,25 @@
       </c>
       <c r="C243" s="7" t="inlineStr">
         <is>
-          <t>Hanna Haugsvær</t>
+          <t>Maria Døske</t>
         </is>
       </c>
       <c r="D243" s="7" t="n">
         <v>2005</v>
       </c>
       <c r="E243" s="15" t="n">
-        <v>11.58</v>
+        <v>11.59</v>
       </c>
       <c r="F243" s="7" t="n">
         <v>691</v>
       </c>
       <c r="G243" s="7" t="inlineStr">
         <is>
-          <t>Ulsteinvik</t>
+          <t>Bærum</t>
         </is>
       </c>
       <c r="H243" s="16" t="n">
-        <v>5.02</v>
+        <v>26.08</v>
       </c>
       <c r="J243" s="5" t="n"/>
       <c r="L243" s="14" t="inlineStr">
@@ -41746,32 +41746,30 @@
     <row r="248" ht="13" customHeight="1">
       <c r="B248" s="14" t="inlineStr">
         <is>
-          <t>400m</t>
+          <t>100m</t>
         </is>
       </c>
       <c r="C248" s="7" t="inlineStr">
         <is>
-          <t>Nora Jakobsen</t>
+          <t>Emilie Høyland Schou</t>
         </is>
       </c>
       <c r="D248" s="7" t="n">
-        <v>2007</v>
-      </c>
-      <c r="E248" s="17" t="inlineStr">
-        <is>
-          <t>1,01,79</t>
-        </is>
+        <v>2005</v>
+      </c>
+      <c r="E248" s="15" t="n">
+        <v>13.28</v>
       </c>
       <c r="F248" s="7" t="n">
         <v>624</v>
       </c>
       <c r="G248" s="7" t="inlineStr">
         <is>
-          <t>Sandnes</t>
+          <t>Lillehammer</t>
         </is>
       </c>
       <c r="H248" s="16" t="n">
-        <v>15.05</v>
+        <v>19.06</v>
       </c>
       <c r="J248" s="5" t="n"/>
       <c r="L248" s="14" t="inlineStr">
@@ -41806,30 +41804,32 @@
     <row r="249" ht="13" customHeight="1">
       <c r="B249" s="14" t="inlineStr">
         <is>
-          <t>100m</t>
+          <t>400m</t>
         </is>
       </c>
       <c r="C249" s="7" t="inlineStr">
         <is>
-          <t>Emilie Høyland Schou</t>
+          <t>Nora Jakobsen</t>
         </is>
       </c>
       <c r="D249" s="7" t="n">
-        <v>2005</v>
-      </c>
-      <c r="E249" s="15" t="n">
-        <v>13.28</v>
+        <v>2007</v>
+      </c>
+      <c r="E249" s="17" t="inlineStr">
+        <is>
+          <t>1,01,79</t>
+        </is>
       </c>
       <c r="F249" s="7" t="n">
         <v>624</v>
       </c>
       <c r="G249" s="7" t="inlineStr">
         <is>
-          <t>Lillehammer</t>
+          <t>Sandnes</t>
         </is>
       </c>
       <c r="H249" s="16" t="n">
-        <v>19.06</v>
+        <v>15.05</v>
       </c>
       <c r="J249" s="5" t="n"/>
       <c r="L249" s="14" t="inlineStr">
@@ -42832,30 +42832,30 @@
     <row r="277" ht="13" customHeight="1">
       <c r="B277" s="14" t="inlineStr">
         <is>
-          <t>Lengde</t>
+          <t>Stav</t>
         </is>
       </c>
       <c r="C277" s="7" t="inlineStr">
         <is>
-          <t>Thale Leirfall Bremset</t>
+          <t>Carmen Nilsson Rismark</t>
         </is>
       </c>
       <c r="D277" s="7" t="n">
-        <v>1999</v>
+        <v>2007</v>
       </c>
       <c r="E277" s="15" t="n">
-        <v>6.13</v>
+        <v>2</v>
       </c>
       <c r="F277" s="7" t="n">
-        <v>871</v>
+        <v>427</v>
       </c>
       <c r="G277" s="7" t="inlineStr">
         <is>
-          <t>Ulsteinvik</t>
+          <t>Stjørdal</t>
         </is>
       </c>
       <c r="H277" s="16" t="n">
-        <v>6.02</v>
+        <v>30.09</v>
       </c>
       <c r="J277" s="5" t="n"/>
       <c r="L277" s="14" t="inlineStr">
@@ -42890,30 +42890,30 @@
     <row r="278" ht="13" customHeight="1">
       <c r="B278" s="14" t="inlineStr">
         <is>
-          <t>Kule</t>
+          <t>Lengde</t>
         </is>
       </c>
       <c r="C278" s="7" t="inlineStr">
         <is>
-          <t>Mali Ingeborg Vollan Marstad</t>
+          <t>Thale Leirfall Bremset</t>
         </is>
       </c>
       <c r="D278" s="7" t="n">
-        <v>1997</v>
+        <v>1999</v>
       </c>
       <c r="E278" s="15" t="n">
-        <v>11.48</v>
+        <v>6.13</v>
       </c>
       <c r="F278" s="7" t="n">
-        <v>685</v>
+        <v>871</v>
       </c>
       <c r="G278" s="7" t="inlineStr">
         <is>
-          <t>Stjørdal</t>
+          <t>Ulsteinvik</t>
         </is>
       </c>
       <c r="H278" s="16" t="n">
-        <v>22.09</v>
+        <v>6.02</v>
       </c>
       <c r="J278" s="5" t="n"/>
       <c r="L278" s="14" t="inlineStr">
@@ -42948,22 +42948,22 @@
     <row r="279" ht="13" customHeight="1">
       <c r="B279" s="14" t="inlineStr">
         <is>
-          <t>Diskos</t>
+          <t>Kule</t>
         </is>
       </c>
       <c r="C279" s="7" t="inlineStr">
         <is>
-          <t>Helle M. Aspaas</t>
+          <t>Mali Ingeborg Vollan Marstad</t>
         </is>
       </c>
       <c r="D279" s="7" t="n">
-        <v>2002</v>
+        <v>1997</v>
       </c>
       <c r="E279" s="15" t="n">
-        <v>39</v>
+        <v>11.48</v>
       </c>
       <c r="F279" s="7" t="n">
-        <v>711</v>
+        <v>685</v>
       </c>
       <c r="G279" s="7" t="inlineStr">
         <is>
@@ -42971,7 +42971,7 @@
         </is>
       </c>
       <c r="H279" s="16" t="n">
-        <v>26.06</v>
+        <v>22.09</v>
       </c>
       <c r="J279" s="5" t="n"/>
       <c r="L279" s="14" t="inlineStr">
@@ -43006,22 +43006,22 @@
     <row r="280" ht="13" customHeight="1">
       <c r="B280" s="14" t="inlineStr">
         <is>
-          <t>Slegge</t>
+          <t>Diskos</t>
         </is>
       </c>
       <c r="C280" s="7" t="inlineStr">
         <is>
-          <t>Mali Ingeborg Vollan Marstad</t>
+          <t>Helle M. Aspaas</t>
         </is>
       </c>
       <c r="D280" s="7" t="n">
-        <v>1997</v>
+        <v>2002</v>
       </c>
       <c r="E280" s="15" t="n">
-        <v>36.64</v>
+        <v>39</v>
       </c>
       <c r="F280" s="7" t="n">
-        <v>638</v>
+        <v>711</v>
       </c>
       <c r="G280" s="7" t="inlineStr">
         <is>
@@ -43029,7 +43029,7 @@
         </is>
       </c>
       <c r="H280" s="16" t="n">
-        <v>22.09</v>
+        <v>26.06</v>
       </c>
       <c r="J280" s="5" t="n"/>
       <c r="L280" s="14" t="inlineStr">
@@ -43064,22 +43064,22 @@
     <row r="281" ht="13" customHeight="1">
       <c r="B281" s="14" t="inlineStr">
         <is>
-          <t>Spyd</t>
+          <t>Slegge</t>
         </is>
       </c>
       <c r="C281" s="7" t="inlineStr">
         <is>
-          <t>Maria Børstad Jensen</t>
+          <t>Mali Ingeborg Vollan Marstad</t>
         </is>
       </c>
       <c r="D281" s="7" t="n">
-        <v>1994</v>
+        <v>1997</v>
       </c>
       <c r="E281" s="15" t="n">
-        <v>51.64</v>
+        <v>36.64</v>
       </c>
       <c r="F281" s="7" t="n">
-        <v>880</v>
+        <v>638</v>
       </c>
       <c r="G281" s="7" t="inlineStr">
         <is>
@@ -43087,7 +43087,7 @@
         </is>
       </c>
       <c r="H281" s="16" t="n">
-        <v>29.05</v>
+        <v>22.09</v>
       </c>
       <c r="J281" s="5" t="n"/>
       <c r="L281" s="14" t="inlineStr">
@@ -43120,13 +43120,33 @@
       <c r="T281" s="5" t="n"/>
     </row>
     <row r="282" ht="13" customHeight="1">
-      <c r="B282" s="14" t="n"/>
-      <c r="C282" s="7" t="n"/>
-      <c r="D282" s="7" t="n"/>
-      <c r="E282" s="7" t="n"/>
-      <c r="F282" s="7" t="n"/>
-      <c r="G282" s="7" t="n"/>
-      <c r="H282" s="21" t="n"/>
+      <c r="B282" s="14" t="inlineStr">
+        <is>
+          <t>Spyd</t>
+        </is>
+      </c>
+      <c r="C282" s="7" t="inlineStr">
+        <is>
+          <t>Maria Børstad Jensen</t>
+        </is>
+      </c>
+      <c r="D282" s="7" t="n">
+        <v>1994</v>
+      </c>
+      <c r="E282" s="15" t="n">
+        <v>51.64</v>
+      </c>
+      <c r="F282" s="7" t="n">
+        <v>880</v>
+      </c>
+      <c r="G282" s="7" t="inlineStr">
+        <is>
+          <t>Stjørdal</t>
+        </is>
+      </c>
+      <c r="H282" s="16" t="n">
+        <v>29.05</v>
+      </c>
       <c r="J282" s="5" t="n"/>
       <c r="L282" s="14" t="inlineStr">
         <is>
@@ -43220,7 +43240,7 @@
         </is>
       </c>
       <c r="C285" s="20" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E285" s="19" t="inlineStr">
         <is>
@@ -43228,7 +43248,7 @@
         </is>
       </c>
       <c r="F285" s="20" t="n">
-        <v>9430</v>
+        <v>9857</v>
       </c>
       <c r="J285" s="5" t="n"/>
       <c r="L285" s="19" t="inlineStr">
@@ -44282,7 +44302,7 @@
         </is>
       </c>
       <c r="C308" s="20" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E308" s="19" t="inlineStr">
         <is>
@@ -44290,7 +44310,7 @@
         </is>
       </c>
       <c r="F308" s="20" t="n">
-        <v>18409</v>
+        <v>18836</v>
       </c>
       <c r="J308" s="5" t="n"/>
       <c r="L308" s="19" t="inlineStr">
@@ -44322,7 +44342,7 @@
         </is>
       </c>
       <c r="C310" s="20" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J310" s="5" t="n"/>
       <c r="L310" s="19" t="inlineStr">
@@ -46689,7 +46709,7 @@
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>16452</v>
+        <v>16497</v>
       </c>
       <c r="E6" s="4" t="inlineStr">
         <is>
@@ -50303,32 +50323,32 @@
       <c r="J79" s="5" t="n"/>
       <c r="L79" s="14" t="inlineStr">
         <is>
-          <t>3000m</t>
+          <t>1500m</t>
         </is>
       </c>
       <c r="M79" s="7" t="inlineStr">
         <is>
-          <t>Eva Pasini Friestad</t>
+          <t>Linn Andrea Lindevik</t>
         </is>
       </c>
       <c r="N79" s="7" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="O79" s="17" t="inlineStr">
         <is>
-          <t>10,35,26</t>
+          <t>4,51,59</t>
         </is>
       </c>
       <c r="P79" s="7" t="n">
-        <v>649</v>
+        <v>657</v>
       </c>
       <c r="Q79" s="7" t="inlineStr">
         <is>
-          <t>Bærum</t>
+          <t>Søgne</t>
         </is>
       </c>
       <c r="R79" s="16" t="n">
-        <v>28.08</v>
+        <v>10.09</v>
       </c>
       <c r="T79" s="5" t="n"/>
     </row>
@@ -50365,32 +50385,32 @@
       <c r="J80" s="5" t="n"/>
       <c r="L80" s="14" t="inlineStr">
         <is>
-          <t>800m</t>
+          <t>3000m</t>
         </is>
       </c>
       <c r="M80" s="7" t="inlineStr">
         <is>
-          <t>Linnea Holsen Meier</t>
+          <t>Eva Pasini Friestad</t>
         </is>
       </c>
       <c r="N80" s="7" t="n">
-        <v>1998</v>
+        <v>2005</v>
       </c>
       <c r="O80" s="17" t="inlineStr">
         <is>
-          <t>2,21,80</t>
+          <t>10,35,26</t>
         </is>
       </c>
       <c r="P80" s="7" t="n">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="Q80" s="7" t="inlineStr">
         <is>
-          <t>Kristiansand</t>
+          <t>Bærum</t>
         </is>
       </c>
       <c r="R80" s="16" t="n">
-        <v>7.05</v>
+        <v>28.08</v>
       </c>
       <c r="T80" s="5" t="n"/>
     </row>
@@ -50432,27 +50452,27 @@
       </c>
       <c r="M81" s="7" t="inlineStr">
         <is>
-          <t>Marie Kristine Malmgren</t>
+          <t>Linnea Holsen Meier</t>
         </is>
       </c>
       <c r="N81" s="7" t="n">
-        <v>1995</v>
+        <v>1998</v>
       </c>
       <c r="O81" s="17" t="inlineStr">
         <is>
-          <t>2,22,24</t>
+          <t>2,21,80</t>
         </is>
       </c>
       <c r="P81" s="7" t="n">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="Q81" s="7" t="inlineStr">
         <is>
-          <t>Grimstad</t>
+          <t>Kristiansand</t>
         </is>
       </c>
       <c r="R81" s="16" t="n">
-        <v>17.02</v>
+        <v>7.05</v>
       </c>
       <c r="T81" s="5" t="n"/>
     </row>
@@ -50487,30 +50507,32 @@
       <c r="J82" s="5" t="n"/>
       <c r="L82" s="14" t="inlineStr">
         <is>
-          <t>60m</t>
+          <t>800m</t>
         </is>
       </c>
       <c r="M82" s="7" t="inlineStr">
         <is>
-          <t>Tina Helen Bergem</t>
+          <t>Marie Kristine Malmgren</t>
         </is>
       </c>
       <c r="N82" s="7" t="n">
-        <v>1994</v>
-      </c>
-      <c r="O82" s="15" t="n">
-        <v>8.34</v>
+        <v>1995</v>
+      </c>
+      <c r="O82" s="17" t="inlineStr">
+        <is>
+          <t>2,22,24</t>
+        </is>
       </c>
       <c r="P82" s="7" t="n">
-        <v>636</v>
+        <v>641</v>
       </c>
       <c r="Q82" s="7" t="inlineStr">
         <is>
-          <t>Bærum</t>
+          <t>Grimstad</t>
         </is>
       </c>
       <c r="R82" s="16" t="n">
-        <v>29.01</v>
+        <v>17.02</v>
       </c>
       <c r="T82" s="5" t="n"/>
     </row>
@@ -50522,11 +50544,11 @@
       </c>
       <c r="C83" s="7" t="inlineStr">
         <is>
-          <t>Kaia Morland</t>
+          <t>Charlotte Celine Thorjussen</t>
         </is>
       </c>
       <c r="D83" s="7" t="n">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="E83" s="15" t="n">
         <v>27.52</v>
@@ -50540,35 +50562,35 @@
         </is>
       </c>
       <c r="H83" s="16" t="n">
-        <v>17.02</v>
+        <v>31.05</v>
       </c>
       <c r="J83" s="5" t="n"/>
       <c r="L83" s="14" t="inlineStr">
         <is>
-          <t>Lengde</t>
+          <t>60m</t>
         </is>
       </c>
       <c r="M83" s="7" t="inlineStr">
         <is>
-          <t>Tora Ugland Damsgaard</t>
+          <t>Tina Helen Bergem</t>
         </is>
       </c>
       <c r="N83" s="7" t="n">
-        <v>2005</v>
+        <v>1994</v>
       </c>
       <c r="O83" s="15" t="n">
-        <v>5.07</v>
+        <v>8.34</v>
       </c>
       <c r="P83" s="7" t="n">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="Q83" s="7" t="inlineStr">
         <is>
-          <t>Grimstad</t>
+          <t>Bærum</t>
         </is>
       </c>
       <c r="R83" s="16" t="n">
-        <v>15.05</v>
+        <v>29.01</v>
       </c>
       <c r="T83" s="5" t="n"/>
     </row>
@@ -50608,17 +50630,17 @@
       </c>
       <c r="M84" s="7" t="inlineStr">
         <is>
-          <t>Marie Mollestad</t>
+          <t>Tora Ugland Damsgaard</t>
         </is>
       </c>
       <c r="N84" s="7" t="n">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="O84" s="15" t="n">
-        <v>5.01</v>
+        <v>5.07</v>
       </c>
       <c r="P84" s="7" t="n">
-        <v>620</v>
+        <v>633</v>
       </c>
       <c r="Q84" s="7" t="inlineStr">
         <is>
@@ -50626,7 +50648,7 @@
         </is>
       </c>
       <c r="R84" s="16" t="n">
-        <v>13.03</v>
+        <v>15.05</v>
       </c>
       <c r="T84" s="5" t="n"/>
     </row>
@@ -50661,30 +50683,30 @@
       <c r="J85" s="5" t="n"/>
       <c r="L85" s="14" t="inlineStr">
         <is>
-          <t>Tresteg</t>
+          <t>Lengde</t>
         </is>
       </c>
       <c r="M85" s="7" t="inlineStr">
         <is>
-          <t>Angelina Min</t>
+          <t>Marie Mollestad</t>
         </is>
       </c>
       <c r="N85" s="7" t="n">
-        <v>2004</v>
+        <v>2007</v>
       </c>
       <c r="O85" s="15" t="n">
-        <v>10.56</v>
+        <v>5.01</v>
       </c>
       <c r="P85" s="7" t="n">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="Q85" s="7" t="inlineStr">
         <is>
-          <t>Bærum</t>
+          <t>Grimstad</t>
         </is>
       </c>
       <c r="R85" s="16" t="n">
-        <v>13.02</v>
+        <v>13.03</v>
       </c>
       <c r="T85" s="5" t="n"/>
     </row>
@@ -50719,32 +50741,30 @@
       <c r="J86" s="5" t="n"/>
       <c r="L86" s="14" t="inlineStr">
         <is>
-          <t>1500m</t>
+          <t>Tresteg</t>
         </is>
       </c>
       <c r="M86" s="7" t="inlineStr">
         <is>
-          <t>Linn Andrea Lindevik</t>
+          <t>Angelina Min</t>
         </is>
       </c>
       <c r="N86" s="7" t="n">
         <v>2004</v>
       </c>
-      <c r="O86" s="17" t="inlineStr">
-        <is>
-          <t>4,59,98</t>
-        </is>
+      <c r="O86" s="15" t="n">
+        <v>10.56</v>
       </c>
       <c r="P86" s="7" t="n">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="Q86" s="7" t="inlineStr">
         <is>
-          <t>Kristiansand</t>
+          <t>Bærum</t>
         </is>
       </c>
       <c r="R86" s="16" t="n">
-        <v>18.08</v>
+        <v>13.02</v>
       </c>
       <c r="T86" s="5" t="n"/>
     </row>
@@ -50798,7 +50818,7 @@
         </is>
       </c>
       <c r="P88" s="20" t="n">
-        <v>7860</v>
+        <v>7905</v>
       </c>
       <c r="T88" s="5" t="n"/>
     </row>
@@ -50838,7 +50858,7 @@
         </is>
       </c>
       <c r="P90" s="20" t="n">
-        <v>16452</v>
+        <v>16497</v>
       </c>
       <c r="T90" s="5" t="n"/>
     </row>
@@ -60041,32 +60061,30 @@
     <row r="317" ht="13" customHeight="1">
       <c r="B317" s="14" t="inlineStr">
         <is>
-          <t>400m</t>
+          <t>60m</t>
         </is>
       </c>
       <c r="C317" s="7" t="inlineStr">
         <is>
-          <t>Margrethe Lauritzen</t>
+          <t>Carina Brunsæl</t>
         </is>
       </c>
       <c r="D317" s="7" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E317" s="17" t="inlineStr">
-        <is>
-          <t>1,03,80</t>
-        </is>
+        <v>2007</v>
+      </c>
+      <c r="E317" s="15" t="n">
+        <v>8.6</v>
       </c>
       <c r="F317" s="7" t="n">
         <v>568</v>
       </c>
       <c r="G317" s="7" t="inlineStr">
         <is>
-          <t>Oslo/Bi</t>
+          <t>Steinkjer</t>
         </is>
       </c>
       <c r="H317" s="16" t="n">
-        <v>13.07</v>
+        <v>5.03</v>
       </c>
       <c r="J317" s="5" t="n"/>
       <c r="L317" s="14" t="inlineStr">

</xml_diff>

<commit_message>
Tidsforbedringer. Tilbakestilte resultatene til Rjukan kvinner
</commit_message>
<xml_diff>
--- a/output/Lagserien 2022 1-2. div.xlsx
+++ b/output/Lagserien 2022 1-2. div.xlsx
@@ -2844,20 +2844,20 @@
     <row r="40" ht="13" customHeight="1">
       <c r="B40" s="14" t="inlineStr">
         <is>
-          <t>1500m</t>
+          <t>800m</t>
         </is>
       </c>
       <c r="C40" s="7" t="inlineStr">
         <is>
-          <t>Ibrahim Buras</t>
+          <t>Luca Thompson</t>
         </is>
       </c>
       <c r="D40" s="7" t="n">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="E40" s="17" t="inlineStr">
         <is>
-          <t>3,49,59</t>
+          <t>1,51,84</t>
         </is>
       </c>
       <c r="F40" s="7" t="n">
@@ -2865,11 +2865,11 @@
       </c>
       <c r="G40" s="7" t="inlineStr">
         <is>
-          <t>Jessheim</t>
+          <t>Weinheim/GER</t>
         </is>
       </c>
       <c r="H40" s="16" t="n">
-        <v>2.06</v>
+        <v>28.05</v>
       </c>
       <c r="J40" s="5" t="n"/>
       <c r="L40" s="14" t="inlineStr">
@@ -2904,20 +2904,20 @@
     <row r="41" ht="13" customHeight="1">
       <c r="B41" s="14" t="inlineStr">
         <is>
-          <t>800m</t>
+          <t>1500m</t>
         </is>
       </c>
       <c r="C41" s="7" t="inlineStr">
         <is>
-          <t>Luca Thompson</t>
+          <t>Ibrahim Buras</t>
         </is>
       </c>
       <c r="D41" s="7" t="n">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="E41" s="17" t="inlineStr">
         <is>
-          <t>1,51,84</t>
+          <t>3,49,59</t>
         </is>
       </c>
       <c r="F41" s="7" t="n">
@@ -2925,11 +2925,11 @@
       </c>
       <c r="G41" s="7" t="inlineStr">
         <is>
-          <t>Weinheim/GER</t>
+          <t>Jessheim</t>
         </is>
       </c>
       <c r="H41" s="16" t="n">
-        <v>28.05</v>
+        <v>2.06</v>
       </c>
       <c r="J41" s="5" t="n"/>
       <c r="L41" s="14" t="inlineStr">
@@ -13186,18 +13186,18 @@
         <v>2002</v>
       </c>
       <c r="E282" s="15" t="n">
-        <v>46.27</v>
+        <v>46.29</v>
       </c>
       <c r="F282" s="7" t="n">
         <v>796</v>
       </c>
       <c r="G282" s="7" t="inlineStr">
         <is>
-          <t>Heggedal</t>
+          <t>Røyken</t>
         </is>
       </c>
       <c r="H282" s="16" t="n">
-        <v>9.08</v>
+        <v>15.1</v>
       </c>
       <c r="J282" s="5" t="n"/>
       <c r="L282" s="14" t="n"/>
@@ -13998,30 +13998,30 @@
     <row r="300" ht="13" customHeight="1">
       <c r="B300" s="14" t="inlineStr">
         <is>
-          <t>Høyde u.t</t>
+          <t>Lengde u.t</t>
         </is>
       </c>
       <c r="C300" s="7" t="inlineStr">
         <is>
-          <t>Erlend Bergfjord Næss</t>
+          <t>Sander Feness Armond</t>
         </is>
       </c>
       <c r="D300" s="7" t="n">
-        <v>2002</v>
+        <v>2005</v>
       </c>
       <c r="E300" s="15" t="n">
-        <v>1.37</v>
+        <v>2.74</v>
       </c>
       <c r="F300" s="7" t="n">
         <v>526</v>
       </c>
       <c r="G300" s="7" t="inlineStr">
         <is>
-          <t>Bergen/La</t>
+          <t>Askøy</t>
         </is>
       </c>
       <c r="H300" s="16" t="n">
-        <v>29.03</v>
+        <v>14.03</v>
       </c>
       <c r="J300" s="5" t="n"/>
       <c r="L300" s="14" t="n"/>
@@ -14036,30 +14036,30 @@
     <row r="301" ht="13" customHeight="1">
       <c r="B301" s="14" t="inlineStr">
         <is>
-          <t>Lengde u.t</t>
+          <t>Høyde u.t</t>
         </is>
       </c>
       <c r="C301" s="7" t="inlineStr">
         <is>
-          <t>Sander Feness Armond</t>
+          <t>Erlend Bergfjord Næss</t>
         </is>
       </c>
       <c r="D301" s="7" t="n">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="E301" s="15" t="n">
-        <v>2.74</v>
+        <v>1.37</v>
       </c>
       <c r="F301" s="7" t="n">
         <v>526</v>
       </c>
       <c r="G301" s="7" t="inlineStr">
         <is>
-          <t>Askøy</t>
+          <t>Bergen/La</t>
         </is>
       </c>
       <c r="H301" s="16" t="n">
-        <v>14.03</v>
+        <v>29.03</v>
       </c>
       <c r="J301" s="5" t="n"/>
       <c r="L301" s="14" t="n"/>
@@ -45985,11 +45985,11 @@
       </c>
       <c r="Q348" s="7" t="inlineStr">
         <is>
-          <t>Fana</t>
+          <t>Leikvang</t>
         </is>
       </c>
       <c r="R348" s="16" t="n">
-        <v>27.05</v>
+        <v>19.02</v>
       </c>
       <c r="T348" s="5" t="n"/>
     </row>

</xml_diff>

<commit_message>
fjernet flere resultater fra rjukan kvinner for å lettgjøre beregning
</commit_message>
<xml_diff>
--- a/output/Lagserien 2022 1-2. div.xlsx
+++ b/output/Lagserien 2022 1-2. div.xlsx
@@ -46841,7 +46841,7 @@
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>16497</v>
+        <v>16508</v>
       </c>
       <c r="E7" s="4" t="inlineStr">
         <is>
@@ -51617,30 +51617,30 @@
     <row r="110" ht="13" customHeight="1">
       <c r="B110" s="14" t="inlineStr">
         <is>
-          <t>60m hekk</t>
+          <t>100m hekk</t>
         </is>
       </c>
       <c r="C110" s="7" t="inlineStr">
         <is>
-          <t>Angelina Min</t>
+          <t>Nathalie Ommundsen Johnsen</t>
         </is>
       </c>
       <c r="D110" s="7" t="n">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="E110" s="15" t="n">
-        <v>10.17</v>
+        <v>16.35</v>
       </c>
       <c r="F110" s="7" t="n">
-        <v>575</v>
+        <v>647</v>
       </c>
       <c r="G110" s="7" t="inlineStr">
         <is>
-          <t>Steinkjer</t>
+          <t>Porsgrunn</t>
         </is>
       </c>
       <c r="H110" s="16" t="n">
-        <v>4.03</v>
+        <v>29.05</v>
       </c>
       <c r="J110" s="5" t="n"/>
       <c r="L110" s="14" t="inlineStr">
@@ -51675,7 +51675,7 @@
     <row r="111" ht="13" customHeight="1">
       <c r="B111" s="14" t="inlineStr">
         <is>
-          <t>100m hekk</t>
+          <t>Lengde</t>
         </is>
       </c>
       <c r="C111" s="7" t="inlineStr">
@@ -51687,18 +51687,18 @@
         <v>1998</v>
       </c>
       <c r="E111" s="15" t="n">
-        <v>16.35</v>
+        <v>5.28</v>
       </c>
       <c r="F111" s="7" t="n">
-        <v>647</v>
+        <v>679</v>
       </c>
       <c r="G111" s="7" t="inlineStr">
         <is>
-          <t>Porsgrunn</t>
+          <t>Nadderud</t>
         </is>
       </c>
       <c r="H111" s="16" t="n">
-        <v>29.05</v>
+        <v>11.06</v>
       </c>
       <c r="J111" s="5" t="n"/>
       <c r="L111" s="14" t="inlineStr">
@@ -51735,30 +51735,30 @@
     <row r="112" ht="13" customHeight="1">
       <c r="B112" s="14" t="inlineStr">
         <is>
-          <t>Lengde</t>
+          <t>Tresteg</t>
         </is>
       </c>
       <c r="C112" s="7" t="inlineStr">
         <is>
-          <t>Nathalie Ommundsen Johnsen</t>
+          <t>Tora Ugland Damsgaard</t>
         </is>
       </c>
       <c r="D112" s="7" t="n">
-        <v>1998</v>
+        <v>2005</v>
       </c>
       <c r="E112" s="15" t="n">
-        <v>5.28</v>
+        <v>10.67</v>
       </c>
       <c r="F112" s="7" t="n">
-        <v>679</v>
+        <v>627</v>
       </c>
       <c r="G112" s="7" t="inlineStr">
         <is>
-          <t>Nadderud</t>
+          <t>Trondheim</t>
         </is>
       </c>
       <c r="H112" s="16" t="n">
-        <v>11.06</v>
+        <v>12.08</v>
       </c>
       <c r="J112" s="5" t="n"/>
       <c r="L112" s="14" t="inlineStr">
@@ -51793,30 +51793,30 @@
     <row r="113" ht="13" customHeight="1">
       <c r="B113" s="14" t="inlineStr">
         <is>
-          <t>Tresteg</t>
+          <t>Høyde u.t</t>
         </is>
       </c>
       <c r="C113" s="7" t="inlineStr">
         <is>
-          <t>Tora Ugland Damsgaard</t>
+          <t>Nathalie Ommundsen Johnsen</t>
         </is>
       </c>
       <c r="D113" s="7" t="n">
-        <v>2005</v>
+        <v>1998</v>
       </c>
       <c r="E113" s="15" t="n">
-        <v>10.67</v>
+        <v>1.3</v>
       </c>
       <c r="F113" s="7" t="n">
-        <v>627</v>
+        <v>662</v>
       </c>
       <c r="G113" s="7" t="inlineStr">
         <is>
-          <t>Trondheim</t>
+          <t>Ulsteinvik</t>
         </is>
       </c>
       <c r="H113" s="16" t="n">
-        <v>12.08</v>
+        <v>5.02</v>
       </c>
       <c r="J113" s="5" t="n"/>
       <c r="L113" s="14" t="inlineStr">
@@ -51851,30 +51851,30 @@
     <row r="114" ht="13" customHeight="1">
       <c r="B114" s="14" t="inlineStr">
         <is>
-          <t>Høyde u.t</t>
+          <t>Lengde u.t</t>
         </is>
       </c>
       <c r="C114" s="7" t="inlineStr">
         <is>
-          <t>Nathalie Ommundsen Johnsen</t>
+          <t>Marie Mollestad</t>
         </is>
       </c>
       <c r="D114" s="7" t="n">
-        <v>1998</v>
+        <v>2007</v>
       </c>
       <c r="E114" s="15" t="n">
-        <v>1.3</v>
+        <v>2.43</v>
       </c>
       <c r="F114" s="7" t="n">
-        <v>662</v>
+        <v>586</v>
       </c>
       <c r="G114" s="7" t="inlineStr">
         <is>
-          <t>Ulsteinvik</t>
+          <t>Kristiansand</t>
         </is>
       </c>
       <c r="H114" s="16" t="n">
-        <v>5.02</v>
+        <v>8.119999999999999</v>
       </c>
       <c r="J114" s="5" t="n"/>
       <c r="L114" s="14" t="inlineStr">
@@ -51997,7 +51997,7 @@
         </is>
       </c>
       <c r="F117" s="20" t="n">
-        <v>8592</v>
+        <v>8603</v>
       </c>
       <c r="J117" s="5" t="n"/>
       <c r="L117" s="19" t="inlineStr">
@@ -52897,7 +52897,7 @@
         </is>
       </c>
       <c r="F137" s="20" t="n">
-        <v>16497</v>
+        <v>16508</v>
       </c>
       <c r="J137" s="5" t="n"/>
       <c r="L137" s="19" t="inlineStr">

</xml_diff>